<commit_message>
PROS-5126- ccru - Formula update for Promo Displays KPI
+ some update in top_gaps in SAND
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
@@ -43,6 +43,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AO$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AO$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AO$172</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AO$172</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -54,156 +55,156 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="513">
-  <si>
-    <t>Sorting</t>
-  </si>
-  <si>
-    <t>SAP PoS</t>
-  </si>
-  <si>
-    <t>Channel</t>
-  </si>
-  <si>
-    <t>KPI Type</t>
-  </si>
-  <si>
-    <t>SAP KPI</t>
-  </si>
-  <si>
-    <t>KPI name Eng</t>
-  </si>
-  <si>
-    <t>KPI name Rus</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>Target</t>
-  </si>
-  <si>
-    <t>target_min</t>
-  </si>
-  <si>
-    <t>target_max</t>
-  </si>
-  <si>
-    <t>SKU</t>
-  </si>
-  <si>
-    <t>Values</t>
-  </si>
-  <si>
-    <t>Product Category</t>
-  </si>
-  <si>
-    <t>Brand</t>
-  </si>
-  <si>
-    <t>Logical Operator</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Size</t>
-  </si>
-  <si>
-    <t>Form Factor</t>
-  </si>
-  <si>
-    <t>Zone to include</t>
-  </si>
-  <si>
-    <t>Locations to exclude</t>
-  </si>
-  <si>
-    <t>Locations to include</t>
-  </si>
-  <si>
-    <t>Scenes to include</t>
-  </si>
-  <si>
-    <t>Scenes to exclude</t>
-  </si>
-  <si>
-    <t>Sub locations to include</t>
-  </si>
-  <si>
-    <t>Sub locations to exclude</t>
-  </si>
-  <si>
-    <t>shelf_number</t>
-  </si>
-  <si>
-    <t>Converted?</t>
-  </si>
-  <si>
-    <t>score_func</t>
-  </si>
-  <si>
-    <t>KPI Weight</t>
-  </si>
-  <si>
-    <t>score_min</t>
-  </si>
-  <si>
-    <t>score_max</t>
-  </si>
-  <si>
-    <t>depends on</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Base KPI for TOP 5 GAPs</t>
-  </si>
-  <si>
-    <t>KPI from POS 2016</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>KPI ID</t>
-  </si>
-  <si>
-    <t>Children</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>To include in first calculation?</t>
-  </si>
-  <si>
-    <t>RD38010003</t>
-  </si>
-  <si>
-    <t>Convenience Big</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>STANDARD 1</t>
-  </si>
-  <si>
-    <t>SSD Availability</t>
-  </si>
-  <si>
-    <t>Представленность SSD</t>
-  </si>
-  <si>
-    <t>Weighted Average </t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>2
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2590" uniqueCount="514">
+  <si>
+    <t xml:space="preserve">Sorting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP PoS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP KPI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI name Eng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI name Rus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">target_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logical Operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form Factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zone to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locations to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenes to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub locations to include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub locations to exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shelf_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Converted?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_func</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score_max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depends on</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Base KPI for TOP 5 GAPs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI from POS 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Children</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To include in first calculation?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RD38010003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convenience Big</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Average </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2
 3
 4
 5
@@ -234,308 +235,308 @@
 30</t>
   </si>
   <si>
-    <t>Coca-Cola - 2L</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 2л</t>
-  </si>
-  <si>
-    <t>number of facings</t>
-  </si>
-  <si>
-    <t>OR</t>
-  </si>
-  <si>
-    <t>SKUs</t>
-  </si>
-  <si>
-    <t>Activation, Other</t>
-  </si>
-  <si>
-    <t>Panoramic Photo</t>
-  </si>
-  <si>
-    <t>BINARY</t>
-  </si>
-  <si>
-    <t>Coca-Cola - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>5449000228970, 5449000054227</t>
-  </si>
-  <si>
-    <t>Coca-Cola - 1.5L</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 1.5л</t>
-  </si>
-  <si>
-    <t>Coca-Cola - 0.5L</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 0.5л</t>
-  </si>
-  <si>
-    <t>Coca-Cola - 0.33L</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 0.33л</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Кока-Кола Зеро - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>5449000231659, 5449000133328</t>
-  </si>
-  <si>
-    <t>Fanta Orange - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Фанта Апельсин - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>5449000228963, 5449000006271</t>
-  </si>
-  <si>
-    <t>Sprite - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Спрайт - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>5449000228956, 5449000050939</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero - 1.5L</t>
-  </si>
-  <si>
-    <t>Кока-Кола Зеро - 1.5л</t>
-  </si>
-  <si>
-    <t>Sprite - 2L</t>
-  </si>
-  <si>
-    <t>Спрайт - 2л</t>
-  </si>
-  <si>
-    <t>Fanta Orange - 2L</t>
-  </si>
-  <si>
-    <t>Фанта Апельсин - 2л</t>
-  </si>
-  <si>
-    <t>Sprite - 1.5L</t>
-  </si>
-  <si>
-    <t>Спрайт - 1.5л</t>
-  </si>
-  <si>
-    <t>Schweppes Bitter Lemon - 1.5L</t>
-  </si>
-  <si>
-    <t>Швеппс Биттер Лемон - 1.5л</t>
-  </si>
-  <si>
-    <t>Fanta Orange - 0.5L</t>
-  </si>
-  <si>
-    <t>Фанта Апельсин - 0.5л</t>
-  </si>
-  <si>
-    <t>Sprite - 0.5L</t>
-  </si>
-  <si>
-    <t>Спрайт - 0.5л</t>
-  </si>
-  <si>
-    <t>Sprite - 0.33L</t>
-  </si>
-  <si>
-    <t>Спрайт - 0.33л</t>
-  </si>
-  <si>
-    <t>Fanta Orange - 1.5L</t>
-  </si>
-  <si>
-    <t>Фанта Апельсин - 1.5л</t>
-  </si>
-  <si>
-    <t>Fanta Orange - 0.33L</t>
-  </si>
-  <si>
-    <t>Фанта Апельсин - 0.33л</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero - 0.5L</t>
-  </si>
-  <si>
-    <t>Кока-Кола Зеро - 0.5л</t>
-  </si>
-  <si>
-    <t>Coca-Cola - 0.25L Slim</t>
-  </si>
-  <si>
-    <t>Кока-Кола - 0.25л слим</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero Lemon - 0.5L</t>
-  </si>
-  <si>
-    <t>Кока-Кола Зеро Лемон - 0.5л</t>
-  </si>
-  <si>
-    <t>Sprite Cucumber-Watermelon - 0.5L</t>
-  </si>
-  <si>
-    <t>Спрайт Огурец-Арбуз - 0.5л</t>
-  </si>
-  <si>
-    <t>Fanta Pear - 0.5L</t>
-  </si>
-  <si>
-    <t>Фанта Груша - 0.5л</t>
-  </si>
-  <si>
-    <t>Fanta Citrus - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Фанта Цитрус - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>5449000234179, 5449000213693</t>
-  </si>
-  <si>
-    <t>Schweppes Tonic - 1L</t>
-  </si>
-  <si>
-    <t>Швеппс Тоник - 1л</t>
-  </si>
-  <si>
-    <t>Schweppes Pomegranate - 1.5L</t>
-  </si>
-  <si>
-    <t>Швеппс Гранат - 1.5л</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero Lemon - 0.9L</t>
-  </si>
-  <si>
-    <t>Кока-Кола Зеро Лемон - 0.9л</t>
-  </si>
-  <si>
-    <t>Sprite Cucumber-Watermelon - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Спрайт Огурец-Арбуз - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>5449000241412, 5449000241429</t>
-  </si>
-  <si>
-    <t>Fanta Pear - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Фанта Груша - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>5449000234155, 5449000172235</t>
-  </si>
-  <si>
-    <t>STANDARD 2</t>
-  </si>
-  <si>
-    <t>Water Availability</t>
-  </si>
-  <si>
-    <t>Представленность Воды</t>
-  </si>
-  <si>
-    <t>32
+    <t xml:space="preserve">Coca-Cola - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SKUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activation, Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panoramic Photo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BINARY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000228970, 5449000054227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000231659, 5449000133328</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000228963, 5449000006271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000228956, 5449000050939</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Bitter Lemon - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Биттер Лемон - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Апельсин - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.25L Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола - 0.25л слим</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero Lemon - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро Лемон - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite Cucumber-Watermelon - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт Огурец-Арбуз - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Pear - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Груша - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Citrus - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Цитрус - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000234179, 5449000213693</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Tonic - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Тоник - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schweppes Pomegranate - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Швеппс Гранат - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero Lemon - 0.9L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кока-Кола Зеро Лемон - 0.9л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite Cucumber-Watermelon - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Спрайт Огурец-Арбуз - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000241412, 5449000241429</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Pear - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фанта Груша - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000234155, 5449000172235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Воды</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32
 33
 34
 35
 36</t>
   </si>
   <si>
-    <t>BonAqua Still - 1L</t>
-  </si>
-  <si>
-    <t>БонАква Негаз - 1л</t>
-  </si>
-  <si>
-    <t>BonAqua Still - 0.5L</t>
-  </si>
-  <si>
-    <t>БонАква Негаз - 0.5л</t>
-  </si>
-  <si>
-    <t>BonAqua Viva - Lemon - 0.5L</t>
-  </si>
-  <si>
-    <t>БонАква Вива - Лимон - 0.5л</t>
-  </si>
-  <si>
-    <t>BonAqua Still - 2L</t>
-  </si>
-  <si>
-    <t>БонАква Негаз - 2л</t>
-  </si>
-  <si>
-    <t>BonAqua Still - 0.33L PET</t>
-  </si>
-  <si>
-    <t>БонАква Негаз - 0.33л ПЭТ</t>
-  </si>
-  <si>
-    <t>Energy Availability</t>
-  </si>
-  <si>
-    <t>Представленность Энергетиков</t>
-  </si>
-  <si>
-    <t>38
+    <t xml:space="preserve">BonAqua Still - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Viva - Lemon - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Вива - Лимон - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still - 0.33L PET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">БонАква Негаз - 0.33л ПЭТ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Энергетиков</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38
 39
 40
 41</t>
   </si>
   <si>
-    <t>Burn Original - 0.5L</t>
-  </si>
-  <si>
-    <t>Берн Оригинальный - 0.5л</t>
-  </si>
-  <si>
-    <t>Monster Green - 0.5L</t>
-  </si>
-  <si>
-    <t>Монстер Грин - 0.5л</t>
-  </si>
-  <si>
-    <t>Burn Apple Kiwi - 0.5L</t>
-  </si>
-  <si>
-    <t>Берн Яблоко-Киви - 0.5л</t>
-  </si>
-  <si>
-    <t>Burn Original - 0.33L</t>
-  </si>
-  <si>
-    <t>Берн Оригинальный - 0.33л</t>
-  </si>
-  <si>
-    <t>Tea Availability</t>
-  </si>
-  <si>
-    <t>Представленность Чая</t>
-  </si>
-  <si>
-    <t>43
+    <t xml:space="preserve">Burn Original - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Берн Оригинальный - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster Green - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Монстер Грин - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Apple Kiwi - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Берн Яблоко-Киви - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burn Original - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Берн Оригинальный - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Чая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43
 44
 45
 46
@@ -544,55 +545,55 @@
 49</t>
   </si>
   <si>
-    <t>Fuze Lemon - 0.5L</t>
-  </si>
-  <si>
-    <t>Фьюз Лимон - 0.5л</t>
-  </si>
-  <si>
-    <t>Fuze Lemon - 1L</t>
-  </si>
-  <si>
-    <t>Фьюз Лимон - 1л</t>
-  </si>
-  <si>
-    <t>Fuze Berry - 1L</t>
-  </si>
-  <si>
-    <t>Фьюз Лесн.ягоды - 1л</t>
-  </si>
-  <si>
-    <t>Fuze Green Strawberry-Raspberry - 0.5L</t>
-  </si>
-  <si>
-    <t>Фьюз Зеленый Клубника-Малина - 0.5л</t>
-  </si>
-  <si>
-    <t>Fuze Green Strawberry-Raspberry - 1L</t>
-  </si>
-  <si>
-    <t>Фьюз Зеленый Клубника-Малина - 1л</t>
-  </si>
-  <si>
-    <t>Fuze Berry - 1.5L</t>
-  </si>
-  <si>
-    <t>Фьюз Лесн.ягоды - 1.5л</t>
-  </si>
-  <si>
-    <t>Fuze Lemon - 1.5L</t>
-  </si>
-  <si>
-    <t>Фьюз Лимон - 1.5л</t>
-  </si>
-  <si>
-    <t>Juice Availability</t>
-  </si>
-  <si>
-    <t>Представленность Сока</t>
-  </si>
-  <si>
-    <t>51
+    <t xml:space="preserve">Fuze Lemon - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Лимон - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Lemon - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Лимон - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Berry - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Лесн.ягоды - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Green Strawberry-Raspberry - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Зеленый Клубника-Малина - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Green Strawberry-Raspberry - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Зеленый Клубника-Малина - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Berry - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Лесн.ягоды - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Lemon - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фьюз Лимон - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Представленность Сока</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51
 52
 53
 54
@@ -629,265 +630,265 @@
 85</t>
   </si>
   <si>
-    <t>Dobriy - Apple - 1L</t>
-  </si>
-  <si>
-    <t>Добрый - Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Multifruit - 1L</t>
-  </si>
-  <si>
-    <t>Добрый - Мультифрут - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Orange - 1L</t>
-  </si>
-  <si>
-    <t>Добрый - Апельсин - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Peach-Apple - 1L</t>
-  </si>
-  <si>
-    <t>Добрый - Персик-Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Tomato - 1L</t>
-  </si>
-  <si>
-    <t>Добрый - Томат - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Apple - 2L</t>
-  </si>
-  <si>
-    <t>Добрый - Яблоко - 2л</t>
-  </si>
-  <si>
-    <t>Dobriy - Multifruit - 2L</t>
-  </si>
-  <si>
-    <t>Добрый - Мультифрут - 2л</t>
-  </si>
-  <si>
-    <t>Dobriy - Orange - 2L</t>
-  </si>
-  <si>
-    <t>Добрый - Апельсин - 2л</t>
-  </si>
-  <si>
-    <t>Pulpy - Orange - 0.45L</t>
-  </si>
-  <si>
-    <t>Палпи - Апельсин - 0.45л</t>
-  </si>
-  <si>
-    <t>Dobriy - Apple - 0.2L</t>
-  </si>
-  <si>
-    <t>Добрый - Яблоко - 0.2л</t>
-  </si>
-  <si>
-    <t>Dobriy - Multifruit - 0.2L</t>
-  </si>
-  <si>
-    <t>Добрый - Мультифрут - 0.2л</t>
-  </si>
-  <si>
-    <t>Dobriy - Apple - 0.33L</t>
-  </si>
-  <si>
-    <t>Добрый - Яблоко - 0.33л</t>
-  </si>
-  <si>
-    <t>Dobriy - Multifruit - 0.33L</t>
-  </si>
-  <si>
-    <t>Добрый - Мультифрут - 0.33л</t>
-  </si>
-  <si>
-    <t>Pulpy - Orange - 0.9L</t>
-  </si>
-  <si>
-    <t>Палпи - Апельсин - 0.9л</t>
-  </si>
-  <si>
-    <t>Rich - Orange - 1L</t>
-  </si>
-  <si>
-    <t>Рич - Апельсин - 1л</t>
-  </si>
-  <si>
-    <t>Rich - Apple - 1L</t>
-  </si>
-  <si>
-    <t>Рич - Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Rich - Cherry - 1L</t>
-  </si>
-  <si>
-    <t>Рич - Вишня - 1л</t>
-  </si>
-  <si>
-    <t>Moya Semya - Berry Fruit - 1L</t>
-  </si>
-  <si>
-    <t>Моя Семья - Фруктово-Ягодный - 1л</t>
-  </si>
-  <si>
-    <t>Moya Semya - Apple - 1L</t>
-  </si>
-  <si>
-    <t>Моя Семья - Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Moya Semya - Multifruit - 1L</t>
-  </si>
-  <si>
-    <t>Моя Семья - Мультифрут - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Apple Cloudy - 1L</t>
-  </si>
-  <si>
-    <t>Добрый - Деревенские яблочки - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Peach-Apple - 2L</t>
-  </si>
-  <si>
-    <t>Добрый - Персик-Яблоко - 2л</t>
-  </si>
-  <si>
-    <t>Dobriy - Tomato - 2L</t>
-  </si>
-  <si>
-    <t>Добрый - Томат - 2л</t>
-  </si>
-  <si>
-    <t>Dobriy - Bodriy Citrus - 1L</t>
-  </si>
-  <si>
-    <t>Добрый - Бодрый Цитрус - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Pomegranate-Grape - 1L</t>
-  </si>
-  <si>
-    <t>Добрый Уголки - Гранат-Виноград - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Pear - 1L</t>
-  </si>
-  <si>
-    <t>Добрый Уголки - Груша - 1л</t>
-  </si>
-  <si>
-    <t>Pulpy - Mango Pineapple - 0.45L</t>
-  </si>
-  <si>
-    <t>Палпи - Манго Ананас - 0.45л</t>
-  </si>
-  <si>
-    <t>Dobriy - Pouch smoothie1 - 0.11L</t>
-  </si>
-  <si>
-    <t>Добрый - Смузи 1 - 0.11л</t>
-  </si>
-  <si>
-    <t>Dobriy - Vegetable Mix - 1L</t>
-  </si>
-  <si>
-    <t>Добрый Уголки - Овощной микс - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Pouch smoothie2 - 0.11L</t>
-  </si>
-  <si>
-    <t>Добрый - Смузи 2 - 0.11л</t>
-  </si>
-  <si>
-    <t>Pulpy - Tropical - 0.45L</t>
-  </si>
-  <si>
-    <t>Палпи - Тропик - 0.45л</t>
-  </si>
-  <si>
-    <t>Moya Semya - Citrus Mix - 1L</t>
-  </si>
-  <si>
-    <t>Моя Семья - Цитрус микс - 1л</t>
-  </si>
-  <si>
-    <t>Rich - Mango-Orange - 1L</t>
-  </si>
-  <si>
-    <t>Рич - Манго-Апельсин - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Peach-Apple - 0.2L</t>
-  </si>
-  <si>
-    <t>Добрый - Персик-Яблоко - 0.2л</t>
-  </si>
-  <si>
-    <t>Dobriy - Orange - 0.33L</t>
-  </si>
-  <si>
-    <t>Добрый - Апельсин - 0.33л</t>
-  </si>
-  <si>
-    <t>STANDARD 20</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Shelf share</t>
-  </si>
-  <si>
-    <t>SSD полка: Доля полки</t>
-  </si>
-  <si>
-    <t>SOS</t>
-  </si>
-  <si>
-    <t>Manufacturer: TCCC</t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t>MAN in CAT</t>
-  </si>
-  <si>
-    <t>Warm Shelf</t>
-  </si>
-  <si>
-    <t>PROPORTIONAL</t>
-  </si>
-  <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Top Shelf</t>
-  </si>
-  <si>
-    <t>SSD полка: Золотая Полка</t>
-  </si>
-  <si>
-    <t>number of atomic KPI Passed</t>
-  </si>
-  <si>
-    <t>AND</t>
-  </si>
-  <si>
-    <t>2, 3</t>
-  </si>
-  <si>
-    <t>88
+    <t xml:space="preserve">Dobriy - Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Multifruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Мультифрут - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Orange - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Апельсин - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Peach-Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Персик-Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Tomato - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Томат - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Apple - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Яблоко - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Multifruit - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Мультифрут - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Orange - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Апельсин - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulpy - Orange - 0.45L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Палпи - Апельсин - 0.45л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Apple - 0.2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Яблоко - 0.2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Multifruit - 0.2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Мультифрут - 0.2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Apple - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Яблоко - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Multifruit - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Мультифрут - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulpy - Orange - 0.9L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Палпи - Апельсин - 0.9л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Orange - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Апельсин - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Cherry - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Вишня - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moya Semya - Berry Fruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Моя Семья - Фруктово-Ягодный - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moya Semya - Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Моя Семья - Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moya Semya - Multifruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Моя Семья - Мультифрут - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Apple Cloudy - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Деревенские яблочки - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Peach-Apple - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Персик-Яблоко - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Tomato - 2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Томат - 2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Bodriy Citrus - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Бодрый Цитрус - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Pomegranate-Grape - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый Уголки - Гранат-Виноград - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Pear - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый Уголки - Груша - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulpy - Mango Pineapple - 0.45L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Палпи - Манго Ананас - 0.45л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Pouch smoothie1 - 0.11L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Смузи 1 - 0.11л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Vegetable Mix - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый Уголки - Овощной микс - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Pouch smoothie2 - 0.11L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Смузи 2 - 0.11л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pulpy - Tropical - 0.45L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Палпи - Тропик - 0.45л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moya Semya - Citrus Mix - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Моя Семья - Цитрус микс - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rich - Mango-Orange - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Рич - Манго-Апельсин - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Peach-Apple - 0.2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Персик-Яблоко - 0.2л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Orange - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Добрый - Апельсин - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Shelf share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Доля полки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manufacturer: TCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAN in CAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warm Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROPORTIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Top Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Золотая Полка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of atomic KPI Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2, 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">88
 89
 90
 91
@@ -896,584 +897,587 @@
 94</t>
   </si>
   <si>
-    <t>Shelf: SKU on Eye level</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Coca-Cola - 0.5L</t>
-  </si>
-  <si>
-    <t>SSD полка: Кока-Кола - 0.5л</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Sprite - 0.5L</t>
-  </si>
-  <si>
-    <t>SSD полка: Спрайт - 0.5л</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Fanta Orange - 0.5L</t>
-  </si>
-  <si>
-    <t>SSD полка: Фанта Апельсин - 0.5л</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Coca-Cola Zero - 0.5L</t>
-  </si>
-  <si>
-    <t>SSD полка: Кока-Кола Зеро - 0.5л</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Coca-Cola - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>SSD полка: Кока-Кола - 0.9/1л</t>
-  </si>
-  <si>
-    <t>Coca-Cola - 0.9L, Coca-Cola - 1L</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Sprite - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>SSD полка: Спрайт - 0.9/1л</t>
-  </si>
-  <si>
-    <t>Sprite - 0.9L, Sprite - 1L</t>
-  </si>
-  <si>
-    <t>SSD Shelf: Fanta Orange - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>SSD полка: Фанта Апельсин - 0.9/1л</t>
-  </si>
-  <si>
-    <t>Fanta Orange - 0.9L, Fanta Orange - 1L</t>
-  </si>
-  <si>
-    <t>STANDARD 23</t>
-  </si>
-  <si>
-    <t>Juice Shelf: Shelf share</t>
-  </si>
-  <si>
-    <t>Сок полка: Доля полки</t>
-  </si>
-  <si>
-    <t>Juices</t>
-  </si>
-  <si>
-    <t>Juice Shelf: Top Shelf</t>
-  </si>
-  <si>
-    <t>Сок полка: Золотая Полка</t>
-  </si>
-  <si>
-    <t>97
+    <t xml:space="preserve">Shelf: SKU on Eye level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Coca-Cola - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Кока-Кола - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Sprite - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Спрайт - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Fanta Orange - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Фанта Апельсин - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Coca-Cola Zero - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Кока-Кола Зеро - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Coca-Cola - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Кока-Кола - 0.9/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola - 0.9L, Coca-Cola - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Sprite - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Спрайт - 0.9/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprite - 0.9L, Sprite - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Shelf: Fanta Orange - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD полка: Фанта Апельсин - 0.9/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fanta Orange - 0.9L, Fanta Orange - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Shelf: Shelf share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок полка: Доля полки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Shelf: Top Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок полка: Золотая Полка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">97
 98
 99
 100
 101</t>
   </si>
   <si>
-    <t>Juice Shelf: Dobriy - Apple - 1L</t>
-  </si>
-  <si>
-    <t>Сок полка: Добрый - Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Juice Shelf: Dobriy - Multifruit - 1L</t>
-  </si>
-  <si>
-    <t>Сок полка: Добрый - Мультифрут - 1л</t>
-  </si>
-  <si>
-    <t>Juice Shelf: Dobriy - Orange - 1L</t>
-  </si>
-  <si>
-    <t>Сок полка: Добрый - Апельсин - 1л</t>
-  </si>
-  <si>
-    <t>Juice Shelf: Moya Semya - Berry Fruit - 1L</t>
-  </si>
-  <si>
-    <t>Сок полка: Моя Семья - Фруктово-Ягодный - 1л</t>
-  </si>
-  <si>
-    <t>Juice Shelf: Moya Semya - Apple - 1L</t>
-  </si>
-  <si>
-    <t>Сок полка: Моя Семья - Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>STANDARD 21</t>
-  </si>
-  <si>
-    <t>Water Shelf: Shelf share</t>
-  </si>
-  <si>
-    <t>Вода полка: Доля полки</t>
-  </si>
-  <si>
-    <t>Water</t>
-  </si>
-  <si>
-    <t>Water Shelf: Top Shelf</t>
-  </si>
-  <si>
-    <t>Вода полка: Золотая Полка</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>Water Shelf: BonAqua Still 1L</t>
-  </si>
-  <si>
-    <t>Вода полка: БонАква Негаз - 1л</t>
-  </si>
-  <si>
-    <t>BonAqua Still 1L</t>
-  </si>
-  <si>
-    <t>STANDARD 24</t>
-  </si>
-  <si>
-    <t>Ice Tea Shelf: Shelf share</t>
-  </si>
-  <si>
-    <t>Холодный Чай полка: Доля полки</t>
-  </si>
-  <si>
-    <t>ice tea</t>
-  </si>
-  <si>
-    <t>Ice Tea Shelf: Top Shelf</t>
-  </si>
-  <si>
-    <t>Холодный Чай полка: Золотая Полка</t>
-  </si>
-  <si>
-    <t>107
+    <t xml:space="preserve">Juice Shelf: Dobriy - Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок полка: Добрый - Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Shelf: Dobriy - Multifruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок полка: Добрый - Мультифрут - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Shelf: Dobriy - Orange - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок полка: Добрый - Апельсин - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Shelf: Moya Semya - Berry Fruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок полка: Моя Семья - Фруктово-Ягодный - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Shelf: Moya Semya - Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок полка: Моя Семья - Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Shelf: Shelf share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вода полка: Доля полки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Shelf: Top Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вода полка: Золотая Полка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Shelf: BonAqua Still 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вода полка: БонАква Негаз - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BonAqua Still 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Tea Shelf: Shelf share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодный Чай полка: Доля полки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ice tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Tea Shelf: Top Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодный Чай полка: Золотая Полка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">107
 108</t>
   </si>
   <si>
-    <t>Ice Tea Shelf: Fuze Lemon - 1L</t>
-  </si>
-  <si>
-    <t>Холодный Чай полка: Фьюз Лимон - 1л</t>
-  </si>
-  <si>
-    <t>Ice Tea Shelf: Fuze Berry - 1L</t>
-  </si>
-  <si>
-    <t>Холодный Чай полка: Фьюз Лесн.ягоды - 1л</t>
-  </si>
-  <si>
-    <t>STANDARD 25</t>
-  </si>
-  <si>
-    <t>Energy Shelf: Shelf share</t>
-  </si>
-  <si>
-    <t>Энергетики полка: Доля полки</t>
-  </si>
-  <si>
-    <t>Energy</t>
-  </si>
-  <si>
-    <t>STANDARD 19</t>
-  </si>
-  <si>
-    <t>SSD Display 1st</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й</t>
-  </si>
-  <si>
-    <t>number of atomic KPI Passed on the same scene</t>
-  </si>
-  <si>
-    <t>SSD Displays</t>
-  </si>
-  <si>
-    <t>111
+    <t xml:space="preserve">Ice Tea Shelf: Fuze Lemon - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодный Чай полка: Фьюз Лимон - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice Tea Shelf: Fuze Berry - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодный Чай полка: Фьюз Лесн.ягоды - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy Shelf: Shelf share</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Энергетики полка: Доля полки</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of atomic KPI Passed on the same scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Displays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111
 112
 113</t>
   </si>
   <si>
-    <t>SSD Display 1st: Facings</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й: Фейсинги</t>
-  </si>
-  <si>
-    <t>SSD Display 1st: Zone</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й: Зона</t>
-  </si>
-  <si>
-    <t>number of scenes</t>
-  </si>
-  <si>
-    <t>SCENES</t>
-  </si>
-  <si>
-    <t>1/3 of the Store</t>
-  </si>
-  <si>
-    <t>SSD Display 1st: Lead SKU Coca-Cola - 1.5L</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й: Основной СКЮ Кока-Кола - 1.5л</t>
-  </si>
-  <si>
-    <t>Lead SKU</t>
-  </si>
-  <si>
-    <t>Coca-Cola 1.5L share on Display. The competitors are only SSD SKUs</t>
-  </si>
-  <si>
-    <t>SSD Display 1st: Merch. Standard</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й: Мерч. Стандарт</t>
-  </si>
-  <si>
-    <t>Checked only for scene that passed SSD Display 1st</t>
-  </si>
-  <si>
-    <t>115
+    <t xml:space="preserve">SSD Display 1st: Facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й: Фейсинги</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st: Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й: Зона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of scenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCENES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/3 of the Store</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st: Lead SKU Coca-Cola - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й: Основной СКЮ Кока-Кола - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead SKU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola 1.5L share on Display. The competitors are only SSD SKUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st: Merch. Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й: Мерч. Стандарт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checked only for scene that passed SSD Display 1st</t>
+  </si>
+  <si>
+    <t xml:space="preserve">115
 116
 117</t>
   </si>
   <si>
-    <t>SSD Display 1st: Coca-Cola - 1.5L</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й: Кока-Кола - 1.5л</t>
-  </si>
-  <si>
-    <t>SSD Display 1st: Sprite - 1.5L</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й: Спрайт - 1.5л</t>
-  </si>
-  <si>
-    <t>SSD Display 1st: Fanta Orange - 1.5L</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 1-й: Фанта Апельсин - 1.5л</t>
-  </si>
-  <si>
-    <t>SSD Display 2d</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 2-й</t>
-  </si>
-  <si>
-    <t>119
+    <t xml:space="preserve">SSD Display 1st: Coca-Cola - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й: Кока-Кола - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st: Sprite - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й: Спрайт - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 1st: Fanta Orange - 1.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 1-й: Фанта Апельсин - 1.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 2-й</t>
+  </si>
+  <si>
+    <t xml:space="preserve">119
 120
 121</t>
   </si>
   <si>
-    <t>SSD Display 2d: Facings</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 2-й: Фейсинги</t>
-  </si>
-  <si>
-    <t>SSD Display 2d: Zone</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 2-й: Зона</t>
-  </si>
-  <si>
-    <t>Bakery</t>
-  </si>
-  <si>
-    <t>SSD Display 2d: Lead SKU Coca-Cola - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 2-й: Основной СКЮ Кока-Кола - 0.9/1л</t>
-  </si>
-  <si>
-    <t>Coca-Cola 0.9L/1L share on Display. The competitors are only SSD SKUs</t>
-  </si>
-  <si>
-    <t>SSD Display 2d: Merch. Standard</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 2-й: Мерч. Стандарт</t>
-  </si>
-  <si>
-    <t>Checked only for scene that passed SSD Display 2d</t>
-  </si>
-  <si>
-    <t>123
+    <t xml:space="preserve">SSD Display 2d: Facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 2-й: Фейсинги</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 2d: Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 2-й: Зона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bakery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 2d: Lead SKU Coca-Cola - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 2-й: Основной СКЮ Кока-Кола - 0.9/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola 0.9L/1L share on Display. The competitors are only SSD SKUs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 2d: Merch. Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 2-й: Мерч. Стандарт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checked only for scene that passed SSD Display 2d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123
 124</t>
   </si>
   <si>
-    <t>SSD Display 2d: Coca-Cola - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 2-й: Кока-Кола - 0.9/1л</t>
-  </si>
-  <si>
-    <t>SSD Display 2d: Coca-Cola Zero - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>SSD Дисплей 2-й: Кока-Кола Зеро - 0.9/1л</t>
-  </si>
-  <si>
-    <t>Coca-Cola Zero - 0.9L, Coca-Cola Zero - 1L</t>
-  </si>
-  <si>
-    <t>Juice Display 1st</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й</t>
-  </si>
-  <si>
-    <t>Juice Displays</t>
-  </si>
-  <si>
-    <t>126
+    <t xml:space="preserve">SSD Display 2d: Coca-Cola - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 2-й: Кока-Кола - 0.9/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Display 2d: Coca-Cola Zero - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD Дисплей 2-й: Кока-Кола Зеро - 0.9/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coca-Cola Zero - 0.9L, Coca-Cola Zero - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Displays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126
 127
 128</t>
   </si>
   <si>
-    <t>Juice Display 1st: Facings</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Фейсинги</t>
-  </si>
-  <si>
-    <t>Juice Display 1st: Zone</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Зона</t>
-  </si>
-  <si>
-    <t>Produce</t>
-  </si>
-  <si>
-    <t>Juice Display 1st: Lead SKU Dobriy - Apple/Multifruit - 1L</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Основной СКЮ Добрый Яблоко/Мультифрут - 1л</t>
-  </si>
-  <si>
-    <t>number of sub atomic KPI Passed</t>
-  </si>
-  <si>
-    <t>129
+    <t xml:space="preserve">Juice Display 1st: Facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Фейсинги</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st: Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Зона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st: Lead SKU Dobriy - Apple/Multifruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Основной СКЮ Добрый Яблоко/Мультифрут - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of sub atomic KPI Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">129
 130</t>
   </si>
   <si>
-    <t>Juice Display 1st: Lead Dobriy - Apple - 1L</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Основной Добрый - Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Apple - 1L share on Display</t>
-  </si>
-  <si>
-    <t>Juice Display 1st: Lead Dobriy - Multifruit - 1L</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Основной Добрый - Мультифрут - 1л</t>
-  </si>
-  <si>
-    <t>Dobriy - Multifruit - 1L share on Display</t>
-  </si>
-  <si>
-    <t>Juice Display 1st: Merch. Standard</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Мерч. Стандарт</t>
-  </si>
-  <si>
-    <t>Checked only for scene that passed Juice Diaplsy 1st</t>
-  </si>
-  <si>
-    <t>132
+    <t xml:space="preserve">Juice Display 1st: Lead Dobriy - Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Основной Добрый - Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Apple - 1L share on Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st: Lead Dobriy - Multifruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Основной Добрый - Мультифрут - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Multifruit - 1L share on Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st: Merch. Standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Мерч. Стандарт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checked only for scene that passed Juice Diaplsy 1st</t>
+  </si>
+  <si>
+    <t xml:space="preserve">132
 133
 134
 135</t>
   </si>
   <si>
-    <t>Juice Display 1st: Dobriy - Apple - 1L</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Добрый - Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Juice Display 1st: Dobriy - Multifruit - 1L</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Добрый - Мультифрут - 1л</t>
-  </si>
-  <si>
-    <t>Juice Display 1st: Dobriy - Orange - 1L</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Добрый - Апельсин - 1л</t>
-  </si>
-  <si>
-    <t>Juice Display 1st: Dobriy - Peach-Apple - 1L</t>
-  </si>
-  <si>
-    <t>Сок Дисплей 1-й: Добрый - Персик-Яблоко - 1л</t>
-  </si>
-  <si>
-    <t>Tea Display</t>
-  </si>
-  <si>
-    <t>Чай Дисплей</t>
-  </si>
-  <si>
-    <t>Tea Displays</t>
-  </si>
-  <si>
-    <t>137
+    <t xml:space="preserve">Juice Display 1st: Dobriy - Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Добрый - Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st: Dobriy - Multifruit - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Добрый - Мультифрут - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st: Dobriy - Orange - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Добрый - Апельсин - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juice Display 1st: Dobriy - Peach-Apple - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сок Дисплей 1-й: Добрый - Персик-Яблоко - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чай Дисплей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Displays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">137
 138
 139</t>
   </si>
   <si>
-    <t>Tea Display: Facings</t>
-  </si>
-  <si>
-    <t>Чай Дисплей: Фейсинги</t>
-  </si>
-  <si>
-    <t>Tea Display: Zone</t>
-  </si>
-  <si>
-    <t>Чай Дисплей: Зона</t>
-  </si>
-  <si>
-    <t>Confectionary/Biscuits section</t>
-  </si>
-  <si>
-    <t>Tea Display: Lead SKU Fuze Berry/Lemon - 1L</t>
-  </si>
-  <si>
-    <t>Чай Дисплей: Основной СКЮ Фьюз Лесн.ягоды/Лимон - 1л</t>
-  </si>
-  <si>
-    <t>140
+    <t xml:space="preserve">Tea Display: Facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чай Дисплей: Фейсинги</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Display: Zone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чай Дисплей: Зона</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confectionary/Biscuits section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Display: Lead SKU Fuze Berry/Lemon - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чай Дисплей: Основной СКЮ Фьюз Лесн.ягоды/Лимон - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">140
 141</t>
   </si>
   <si>
-    <t>Tea Display: Lead Fuze Lemon - 1L</t>
-  </si>
-  <si>
-    <t>Чай Дисплей: Основной Фьюз Лимон - 1л</t>
-  </si>
-  <si>
-    <t>Fuze Lemon - 1L share on Display</t>
-  </si>
-  <si>
-    <t>Tea Display: Lead SKU Fuze Lemon/Berry - 1L</t>
-  </si>
-  <si>
-    <t>Tea Display: Lead Fuze Berry - 1L</t>
-  </si>
-  <si>
-    <t>Чай Дисплей: Основной Фьюз Лесн.ягоды - 1л</t>
-  </si>
-  <si>
-    <t>Fuze Berry - 1L share on Display</t>
-  </si>
-  <si>
-    <t>STANDARD 22</t>
-  </si>
-  <si>
-    <t>Cooler: Doors</t>
-  </si>
-  <si>
-    <t>Холодильники: Количество Дверей</t>
-  </si>
-  <si>
-    <t>sum of atomic KPI result</t>
-  </si>
-  <si>
-    <t>Plus</t>
-  </si>
-  <si>
-    <t>Store Master Data attr15</t>
-  </si>
-  <si>
-    <t>143
+    <t xml:space="preserve">Tea Display: Lead Fuze Lemon - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чай Дисплей: Основной Фьюз Лимон - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Lemon - 1L share on Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Display: Lead SKU Fuze Lemon/Berry - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea Display: Lead Fuze Berry - 1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Чай Дисплей: Основной Фьюз Лесн.ягоды - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fuze Berry - 1L share on Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STANDARD 22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Количество Дверей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sum of atomic KPI result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store Master Data attr15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">143
 144</t>
   </si>
   <si>
-    <t>Cooler: CCH Cooler Doors</t>
-  </si>
-  <si>
-    <t>Холодильники: Количество Дверей Холодильников Компании</t>
-  </si>
-  <si>
-    <t>number of coolers with facings target and fullness target</t>
-  </si>
-  <si>
-    <t>TCCC</t>
-  </si>
-  <si>
-    <t>MAN</t>
-  </si>
-  <si>
-    <t>Cooler</t>
-  </si>
-  <si>
-    <t>Cooler: Customer Cooler Doors</t>
-  </si>
-  <si>
-    <t>Холодильники: Количество Дверей Холодильников Клиента</t>
-  </si>
-  <si>
-    <t>facings TCCC/40</t>
-  </si>
-  <si>
-    <t>Other Coolers, Cold Shelf</t>
-  </si>
-  <si>
-    <t>Cooler: Prime Position</t>
-  </si>
-  <si>
-    <t>Холодильники: Лучшее место</t>
-  </si>
-  <si>
-    <t>NUM_SCENES</t>
-  </si>
-  <si>
-    <t>1/3 of the Store, Beverage Section, Regular checkouts, Bakery</t>
-  </si>
-  <si>
-    <t>Calculate only for doors that were passed KPI "Cooler: CCH Cooler Doors"</t>
-  </si>
-  <si>
-    <t>CCH coolers quality (Prime Pos, Max15, Merch STD, Occupancy, Lights&amp;clean)</t>
-  </si>
-  <si>
-    <t>Cooler: Max 23</t>
-  </si>
-  <si>
-    <t>Холодильники: Максимум 23 СКЮ на дверь</t>
-  </si>
-  <si>
-    <t>number of SKU per Door RANGE</t>
-  </si>
-  <si>
-    <t>Cooler: Merch Priorty STD</t>
-  </si>
-  <si>
-    <t>Холодильники: Мерч. Стандарты</t>
-  </si>
-  <si>
-    <t>148
+    <t xml:space="preserve">Cooler: CCH Cooler Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Количество Дверей Холодильников Компании</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of coolers with facings target and fullness target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCCC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Customer Cooler Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Количество Дверей Холодильников Клиента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facings TCCC/40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other Coolers, Cold Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Prime Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Лучшее место</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUM_SCENES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/3 of the Store, Beverage Section, Regular checkouts, Bakery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate only for doors that were passed KPI "Cooler: CCH Cooler Doors"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCH coolers quality (Prime Pos, Max15, Merch STD, Occupancy, Lights&amp;clean)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Max 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Максимум 23 СКЮ на дверь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of SKU per Door RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Merch Priorty STD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Мерч. Стандарты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONDITIONAL PROPORTIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">148
 149
 150
 151
@@ -1491,229 +1495,229 @@
 163</t>
   </si>
   <si>
-    <t>Cooler: BonAqua Still - 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: БонАква Негаз - 0.5л</t>
-  </si>
-  <si>
-    <t>Cooler: Burn Original - 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Берн Оригинальный - 0.5л</t>
-  </si>
-  <si>
-    <t>Cooler: Coca-Cola - 0.33L</t>
-  </si>
-  <si>
-    <t>Холодильники: Кока-Кола - 0.33л</t>
-  </si>
-  <si>
-    <t>Cooler: Coca-Cola - 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Кока-Кола - 0.5л</t>
-  </si>
-  <si>
-    <t>Cooler: Coca-Cola - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Холодильники: Кока-Кола - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>Cooler: Coca-Cola Zero - 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Кока-Кола Зеро - 0.5л</t>
-  </si>
-  <si>
-    <t>Cooler: Coca-Cola Zero - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Холодильники: Кока-Кола Зеро - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>Cooler: Fanta Orange - 0.33L</t>
-  </si>
-  <si>
-    <t>Холодильники: Фанта Апельсин - 0.33л</t>
-  </si>
-  <si>
-    <t>Cooler: Fanta Orange - 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Фанта Апельсин - 0.5л</t>
-  </si>
-  <si>
-    <t>Cooler: Fanta Orange - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Холодильники: Фанта Апельсин - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>Cooler: ANY Fuze Green 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Фьюз Зеленый - 0.5л любой</t>
-  </si>
-  <si>
-    <t>ANY Fuze Green 0.5L</t>
-  </si>
-  <si>
-    <t>5449000233615, 5449000189370</t>
-  </si>
-  <si>
-    <t>Cooler: ANY Fuze Black 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Фьюз Черный - 0.5л любой</t>
-  </si>
-  <si>
-    <t>ANY Fuze Black 0.5L</t>
-  </si>
-  <si>
-    <t>5449000189301, 5449000189332, 5449000193124</t>
-  </si>
-  <si>
-    <t>Cooler: Monster Green - 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Монстер Грин - 0.5л</t>
-  </si>
-  <si>
-    <t>Cooler: Sprite - 0.33L</t>
-  </si>
-  <si>
-    <t>Холодильники: Спрайт - 0.33л</t>
-  </si>
-  <si>
-    <t>Cooler: Sprite - 0.5L</t>
-  </si>
-  <si>
-    <t>Холодильники: Спрайт - 0.5л</t>
-  </si>
-  <si>
-    <t>Cooler: Sprite - 0.9L/1L</t>
-  </si>
-  <si>
-    <t>Холодильники: Спрайт - 0.9л/1л</t>
-  </si>
-  <si>
-    <t>Cooler:  w/o other products</t>
-  </si>
-  <si>
-    <t>Холодильники: Без чужой продукции</t>
-  </si>
-  <si>
-    <t>Share of CCH doors which have 98% TCCC facings</t>
-  </si>
-  <si>
-    <t>Promo Displays</t>
-  </si>
-  <si>
-    <t>Промо дисплеи</t>
-  </si>
-  <si>
-    <t>166</t>
-  </si>
-  <si>
-    <t>Promo displays SAP</t>
-  </si>
-  <si>
-    <t>Promo Displays: Facings</t>
-  </si>
-  <si>
-    <t>Промо дисплеи: Фейсинги</t>
-  </si>
-  <si>
-    <t>check_number_of_scenes_with_facings_target</t>
-  </si>
-  <si>
-    <t>COUNT</t>
-  </si>
-  <si>
-    <t>number of scenes with have at least target amount of facings</t>
-  </si>
-  <si>
-    <t>RGM Activations</t>
-  </si>
-  <si>
-    <t>RGM Активации</t>
-  </si>
-  <si>
-    <t>168
+    <t xml:space="preserve">Cooler: BonAqua Still - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: БонАква Негаз - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Burn Original - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Берн Оригинальный - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Coca-Cola - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Кока-Кола - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Coca-Cola - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Кока-Кола - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Coca-Cola - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Кока-Кола - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Coca-Cola Zero - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Кока-Кола Зеро - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Coca-Cola Zero - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Кока-Кола Зеро - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Fanta Orange - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Фанта Апельсин - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Fanta Orange - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Фанта Апельсин - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Fanta Orange - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Фанта Апельсин - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: ANY Fuze Green 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Фьюз Зеленый - 0.5л любой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANY Fuze Green 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000233615, 5449000189370</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: ANY Fuze Black 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Фьюз Черный - 0.5л любой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANY Fuze Black 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5449000189301, 5449000189332, 5449000193124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Monster Green - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Монстер Грин - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Sprite - 0.33L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Спрайт - 0.33л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Sprite - 0.5L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Спрайт - 0.5л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler: Sprite - 0.9L/1L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Спрайт - 0.9л/1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler:  w/o other products</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холодильники: Без чужой продукции</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of CCH doors which have 98% TCCC facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promo Displays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Промо дисплеи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promo displays SAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promo Displays: Facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Промо дисплеи: Фейсинги</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check_number_of_scenes_with_facings_target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">number of scenes with have at least target amount of facings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Activations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Активации</t>
+  </si>
+  <si>
+    <t xml:space="preserve">168
 169
 170
 171</t>
   </si>
   <si>
-    <t>RGM Activations SAP</t>
-  </si>
-  <si>
-    <t>RGM Activations: SSD with Meal</t>
-  </si>
-  <si>
-    <t>RGM Активации: SSD с едой</t>
-  </si>
-  <si>
-    <t>SSD with Meal</t>
-  </si>
-  <si>
-    <t>RGM Activations: Juice &amp; Meal</t>
-  </si>
-  <si>
-    <t>RGM Активации: Сок с едой</t>
-  </si>
-  <si>
-    <t>Dobriy 0.2L near infant Food, Pulpy 0.45L near Milk, Dobriy 0.33L in Bakery, Rich 1L near Cakes</t>
-  </si>
-  <si>
-    <t>RGM Activations: On-the-go</t>
-  </si>
-  <si>
-    <t>RGM Активации: На ходу</t>
-  </si>
-  <si>
-    <t>On-the-go</t>
-  </si>
-  <si>
-    <t>RGM Activations: Screen time</t>
-  </si>
-  <si>
-    <t>RGM Активации: У Экрана</t>
-  </si>
-  <si>
-    <t>Screen time</t>
-  </si>
-  <si>
-    <t>Number of Doors</t>
-  </si>
-  <si>
-    <t>Facings Target</t>
-  </si>
-  <si>
-    <t>Facing Fact</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Share of TCCC product</t>
-  </si>
-  <si>
-    <t>Target per Door</t>
-  </si>
-  <si>
-    <t>Scene</t>
-  </si>
-  <si>
-    <t>KPI Score Formula</t>
-  </si>
-  <si>
-    <t>KPI weighted Score</t>
-  </si>
-  <si>
-    <t>Will be added on the 16th of December</t>
+    <t xml:space="preserve">RGM Activations SAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Activations: SSD with Meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Активации: SSD с едой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD with Meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Activations: Juice &amp; Meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Активации: Сок с едой</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy 0.2L near infant Food, Pulpy 0.45L near Milk, Dobriy 0.33L in Bakery, Rich 1L near Cakes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Activations: On-the-go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Активации: На ходу</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On-the-go</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Activations: Screen time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Активации: У Экрана</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facings Target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facing Fact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Share of TCCC product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target per Door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI Score Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KPI weighted Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will be added on the 16th of December</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1725,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0%"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
@@ -1963,7 +1967,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="92">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2244,7 +2248,15 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2411,28 +2423,22 @@
   </sheetPr>
   <dimension ref="A1:AP172"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="AC148" activeCellId="0" sqref="AC148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="36" min="18" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="7.81781376518219"/>
-    <col collapsed="false" hidden="false" max="41" min="38" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3238866396761"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.93522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.5263157894737"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="11.8744939271255"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.668016194332"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="7.95546558704453"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="23.2591093117409"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="83.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14788,7 +14794,7 @@
       </c>
       <c r="AO147" s="11"/>
     </row>
-    <row r="148" customFormat="false" ht="260.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="221.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="13" t="n">
         <v>147</v>
       </c>
@@ -14841,14 +14847,18 @@
       <c r="AB148" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="AC148" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD148" s="25" t="n">
+      <c r="AC148" s="70" t="s">
+        <v>438</v>
+      </c>
+      <c r="AD148" s="71" t="n">
         <v>0.0225</v>
       </c>
-      <c r="AE148" s="70"/>
-      <c r="AF148" s="15"/>
+      <c r="AE148" s="72" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AF148" s="55" t="n">
+        <v>1</v>
+      </c>
       <c r="AG148" s="15" t="s">
         <v>417</v>
       </c>
@@ -14864,7 +14874,7 @@
         <v>147</v>
       </c>
       <c r="AM148" s="46" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AN148" s="68" t="s">
         <v>432</v>
@@ -14888,10 +14898,10 @@
         <v>246</v>
       </c>
       <c r="F149" s="15" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G149" s="21" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H149" s="15" t="s">
         <v>52</v>
@@ -14975,10 +14985,10 @@
         <v>246</v>
       </c>
       <c r="F150" s="15" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G150" s="21" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H150" s="15" t="s">
         <v>52</v>
@@ -15062,10 +15072,10 @@
         <v>246</v>
       </c>
       <c r="F151" s="15" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="G151" s="21" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H151" s="15" t="s">
         <v>52</v>
@@ -15149,10 +15159,10 @@
         <v>246</v>
       </c>
       <c r="F152" s="15" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="G152" s="21" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="H152" s="15" t="s">
         <v>52</v>
@@ -15236,10 +15246,10 @@
         <v>246</v>
       </c>
       <c r="F153" s="63" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G153" s="26" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="H153" s="15" t="s">
         <v>52</v>
@@ -15252,7 +15262,7 @@
       <c r="L153" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="M153" s="71" t="s">
+      <c r="M153" s="73" t="s">
         <v>60</v>
       </c>
       <c r="N153" s="37"/>
@@ -15323,10 +15333,10 @@
         <v>246</v>
       </c>
       <c r="F154" s="15" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="G154" s="21" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H154" s="15" t="s">
         <v>52</v>
@@ -15410,10 +15420,10 @@
         <v>246</v>
       </c>
       <c r="F155" s="63" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G155" s="26" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H155" s="15" t="s">
         <v>52</v>
@@ -15426,7 +15436,7 @@
       <c r="L155" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="M155" s="71" t="s">
+      <c r="M155" s="73" t="s">
         <v>69</v>
       </c>
       <c r="N155" s="37"/>
@@ -15497,10 +15507,10 @@
         <v>246</v>
       </c>
       <c r="F156" s="15" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G156" s="21" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H156" s="15" t="s">
         <v>52</v>
@@ -15584,10 +15594,10 @@
         <v>246</v>
       </c>
       <c r="F157" s="15" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="G157" s="21" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H157" s="15" t="s">
         <v>52</v>
@@ -15671,10 +15681,10 @@
         <v>246</v>
       </c>
       <c r="F158" s="63" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="G158" s="26" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H158" s="15" t="s">
         <v>52</v>
@@ -15687,7 +15697,7 @@
       <c r="L158" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="M158" s="71" t="s">
+      <c r="M158" s="73" t="s">
         <v>72</v>
       </c>
       <c r="N158" s="37"/>
@@ -15758,10 +15768,10 @@
         <v>246</v>
       </c>
       <c r="F159" s="15" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="G159" s="21" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="H159" s="15" t="s">
         <v>52</v>
@@ -15772,10 +15782,10 @@
       <c r="J159" s="15"/>
       <c r="K159" s="15"/>
       <c r="L159" s="15" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M159" s="24" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="N159" s="37"/>
       <c r="O159" s="37"/>
@@ -15845,10 +15855,10 @@
         <v>246</v>
       </c>
       <c r="F160" s="15" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="G160" s="21" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="H160" s="15" t="s">
         <v>52</v>
@@ -15859,10 +15869,10 @@
       <c r="J160" s="15"/>
       <c r="K160" s="15"/>
       <c r="L160" s="15" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="M160" s="24" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="N160" s="37"/>
       <c r="O160" s="37"/>
@@ -15932,10 +15942,10 @@
         <v>246</v>
       </c>
       <c r="F161" s="15" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G161" s="21" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="H161" s="15" t="s">
         <v>52</v>
@@ -16019,10 +16029,10 @@
         <v>246</v>
       </c>
       <c r="F162" s="15" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="G162" s="21" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="H162" s="15" t="s">
         <v>52</v>
@@ -16106,10 +16116,10 @@
         <v>246</v>
       </c>
       <c r="F163" s="15" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="G163" s="21" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="H163" s="15" t="s">
         <v>52</v>
@@ -16193,10 +16203,10 @@
         <v>246</v>
       </c>
       <c r="F164" s="63" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G164" s="26" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="H164" s="15" t="s">
         <v>52</v>
@@ -16209,7 +16219,7 @@
       <c r="L164" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="M164" s="71" t="s">
+      <c r="M164" s="73" t="s">
         <v>75</v>
       </c>
       <c r="N164" s="37"/>
@@ -16280,13 +16290,13 @@
         <v>246</v>
       </c>
       <c r="F165" s="15" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G165" s="11" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="H165" s="39" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="I165" s="15"/>
       <c r="J165" s="15"/>
@@ -16359,14 +16369,14 @@
       <c r="D166" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="E166" s="72" t="s">
+      <c r="E166" s="74" t="s">
         <v>246</v>
       </c>
       <c r="F166" s="15" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G166" s="11" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="H166" s="15" t="s">
         <v>413</v>
@@ -16389,7 +16399,7 @@
       <c r="T166" s="15"/>
       <c r="U166" s="15"/>
       <c r="V166" s="15" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="W166" s="15"/>
       <c r="X166" s="15"/>
@@ -16417,11 +16427,11 @@
       <c r="AL166" s="18" t="n">
         <v>165</v>
       </c>
-      <c r="AM166" s="73" t="s">
-        <v>480</v>
+      <c r="AM166" s="75" t="s">
+        <v>481</v>
       </c>
       <c r="AN166" s="68" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="AO166" s="11"/>
     </row>
@@ -16438,17 +16448,17 @@
       <c r="D167" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="E167" s="72" t="s">
+      <c r="E167" s="74" t="s">
         <v>246</v>
       </c>
       <c r="F167" s="15" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="G167" s="11" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="H167" s="66" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="I167" s="66" t="n">
         <v>1</v>
@@ -16476,7 +16486,7 @@
       <c r="T167" s="15"/>
       <c r="U167" s="15"/>
       <c r="V167" s="15" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="W167" s="15"/>
       <c r="X167" s="15"/>
@@ -16487,7 +16497,7 @@
         <v>48</v>
       </c>
       <c r="AC167" s="15" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AD167" s="25" t="n">
         <v>1</v>
@@ -16495,8 +16505,8 @@
       <c r="AE167" s="15"/>
       <c r="AF167" s="15"/>
       <c r="AG167" s="15"/>
-      <c r="AH167" s="74" t="s">
-        <v>486</v>
+      <c r="AH167" s="76" t="s">
+        <v>487</v>
       </c>
       <c r="AI167" s="15"/>
       <c r="AJ167" s="15"/>
@@ -16507,8 +16517,8 @@
         <v>166</v>
       </c>
       <c r="AM167" s="11"/>
-      <c r="AN167" s="75" t="s">
-        <v>478</v>
+      <c r="AN167" s="77" t="s">
+        <v>479</v>
       </c>
       <c r="AO167" s="11"/>
     </row>
@@ -16529,10 +16539,10 @@
         <v>246</v>
       </c>
       <c r="F168" s="15" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="G168" s="11" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="H168" s="15" t="s">
         <v>249</v>
@@ -16582,10 +16592,10 @@
         <v>167</v>
       </c>
       <c r="AM168" s="46" t="s">
-        <v>489</v>
-      </c>
-      <c r="AN168" s="76" t="s">
         <v>490</v>
+      </c>
+      <c r="AN168" s="78" t="s">
+        <v>491</v>
       </c>
       <c r="AO168" s="11"/>
     </row>
@@ -16606,10 +16616,10 @@
         <v>246</v>
       </c>
       <c r="F169" s="15" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="G169" s="11" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H169" s="11" t="s">
         <v>323</v>
@@ -16634,8 +16644,8 @@
       <c r="T169" s="15"/>
       <c r="U169" s="15"/>
       <c r="V169" s="15"/>
-      <c r="W169" s="77" t="s">
-        <v>493</v>
+      <c r="W169" s="79" t="s">
+        <v>494</v>
       </c>
       <c r="X169" s="15"/>
       <c r="Y169" s="16"/>
@@ -16664,7 +16674,7 @@
       </c>
       <c r="AM169" s="15"/>
       <c r="AN169" s="15" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AO169" s="11"/>
     </row>
@@ -16685,10 +16695,10 @@
         <v>246</v>
       </c>
       <c r="F170" s="15" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="G170" s="11" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H170" s="11" t="s">
         <v>323</v>
@@ -16714,7 +16724,7 @@
       <c r="U170" s="15"/>
       <c r="V170" s="15"/>
       <c r="W170" s="6" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="X170" s="15"/>
       <c r="Y170" s="16"/>
@@ -16743,7 +16753,7 @@
       </c>
       <c r="AM170" s="15"/>
       <c r="AN170" s="15" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AO170" s="11"/>
     </row>
@@ -16764,10 +16774,10 @@
         <v>246</v>
       </c>
       <c r="F171" s="15" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G171" s="11" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="H171" s="11" t="s">
         <v>323</v>
@@ -16793,7 +16803,7 @@
       <c r="U171" s="15"/>
       <c r="V171" s="15"/>
       <c r="W171" s="6" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="X171" s="15"/>
       <c r="Y171" s="16"/>
@@ -16822,7 +16832,7 @@
       </c>
       <c r="AM171" s="15"/>
       <c r="AN171" s="15" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AO171" s="11"/>
     </row>
@@ -16843,10 +16853,10 @@
         <v>246</v>
       </c>
       <c r="F172" s="15" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G172" s="11" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="H172" s="11" t="s">
         <v>323</v>
@@ -16872,7 +16882,7 @@
       <c r="U172" s="15"/>
       <c r="V172" s="15"/>
       <c r="W172" s="6" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="X172" s="15"/>
       <c r="Y172" s="16"/>
@@ -16901,7 +16911,7 @@
       </c>
       <c r="AM172" s="15"/>
       <c r="AN172" s="15" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AO172" s="11"/>
     </row>
@@ -16935,17 +16945,14 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="78" t="s">
-        <v>493</v>
+      <c r="A1" s="80" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="81" t="s">
         <v>431</v>
       </c>
     </row>
@@ -16972,41 +16979,38 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="82" t="s">
         <v>417</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="D1" s="0" t="s">
+        <v>505</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>506</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>507</v>
+      </c>
+      <c r="H1" s="82" t="s">
+        <v>476</v>
+      </c>
+      <c r="I1" s="0" t="s">
         <v>504</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>505</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>506</v>
-      </c>
-      <c r="H1" s="80" t="s">
-        <v>475</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>503</v>
-      </c>
       <c r="J1" s="0" t="s">
+        <v>508</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>507</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>506</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="80"/>
+      <c r="B2" s="82"/>
       <c r="C2" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -17014,19 +17018,19 @@
         <f aca="false">C2*$C$6</f>
         <v>19.6</v>
       </c>
-      <c r="E2" s="81" t="n">
+      <c r="E2" s="83" t="n">
         <v>20</v>
       </c>
-      <c r="H2" s="80"/>
+      <c r="H2" s="82"/>
       <c r="I2" s="0" t="n">
         <v>0.7</v>
       </c>
-      <c r="J2" s="82" t="n">
+      <c r="J2" s="84" t="n">
         <v>0.99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="80"/>
+      <c r="B3" s="82"/>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
@@ -17034,19 +17038,19 @@
         <f aca="false">C3*$C$6</f>
         <v>28</v>
       </c>
-      <c r="E3" s="83" t="n">
+      <c r="E3" s="85" t="n">
         <v>22</v>
       </c>
-      <c r="H3" s="80"/>
+      <c r="H3" s="82"/>
       <c r="I3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="84" t="n">
+      <c r="J3" s="86" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="80"/>
+      <c r="B4" s="82"/>
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
@@ -17054,28 +17058,28 @@
         <f aca="false">C4*$C$6</f>
         <v>56</v>
       </c>
-      <c r="E4" s="83" t="n">
+      <c r="E4" s="85" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="85" t="n">
+      <c r="F4" s="87" t="n">
         <f aca="false">C2/SUM(C2:C4)</f>
         <v>0.189189189189189</v>
       </c>
-      <c r="H4" s="80"/>
+      <c r="H4" s="82"/>
       <c r="I4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="82" t="n">
+      <c r="J4" s="84" t="n">
         <v>0.99</v>
       </c>
-      <c r="K4" s="86" t="n">
+      <c r="K4" s="88" t="n">
         <f aca="false">SUM(I2,I4)/SUM(I2:I4)</f>
         <v>0.72972972972973</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>28</v>
@@ -17104,54 +17108,51 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.78542510121457"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="88" t="s">
+      <c r="D1" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="88" t="s">
+      <c r="E1" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="88" t="s">
-        <v>509</v>
-      </c>
-      <c r="H1" s="88" t="s">
+      <c r="G1" s="90" t="s">
         <v>510</v>
       </c>
-      <c r="I1" s="88" t="s">
+      <c r="H1" s="90" t="s">
+        <v>511</v>
+      </c>
+      <c r="I1" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="88" t="s">
+      <c r="J1" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="88" t="s">
-        <v>511</v>
-      </c>
-      <c r="L1" s="88" t="s">
+      <c r="K1" s="90" t="s">
+        <v>512</v>
+      </c>
+      <c r="L1" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="88" t="s">
+      <c r="M1" s="90" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="89" t="s">
-        <v>512</v>
+      <c r="B4" s="91" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROS-5708 SD-42148 - CCRU - KPI update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Convenience Big" sheetId="1" state="visible" r:id="rId2"/>
@@ -49,6 +49,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1572,7 +1574,7 @@
     <t xml:space="preserve">ANY Fuze Green 0.5L</t>
   </si>
   <si>
-    <t xml:space="preserve">5449000233615, 5449000189370</t>
+    <t xml:space="preserve">5449000233615, 5449000189370, 5449000027450</t>
   </si>
   <si>
     <t xml:space="preserve">Cooler: ANY Fuze Black 0.5L</t>
@@ -2484,18 +2486,18 @@
   <dimension ref="A1:AR184"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="O160" activeCellId="0" sqref="O160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="13.9028340080972"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="45.4534412955466"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="13.9028340080972"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.9028340080972"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="13.9028340080972"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="46.2753036437247"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="13.9271255060729"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="13.9271255060729"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="51.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-6118 - CCRU - KPI atomic names fixed in templates
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
@@ -54,6 +54,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -826,7 +827,7 @@
     <t xml:space="preserve">Палпи - Манго Ананас - 0.45л</t>
   </si>
   <si>
-    <t xml:space="preserve">Dobriy - Berry Smoothie – 0.11L</t>
+    <t xml:space="preserve">Dobriy - Berry Smoothie - 0.11L</t>
   </si>
   <si>
     <t xml:space="preserve">Добрый Смуззи - Ягодный Дэнс - 110 гр</t>
@@ -2481,7 +2482,6 @@
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -2559,18 +2559,18 @@
   <dimension ref="A1:AR184"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H94" activeCellId="0" sqref="H94"/>
+      <selection pane="bottomLeft" activeCell="G80" activeCellId="0" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="14.6882591093117"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="49.9473684210526"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="14.6882591093117"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="14.6882591093117"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="14.6882591093117"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="52.2753036437247"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="15.2834008097166"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="51.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18430,7 +18430,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18467,7 +18467,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18599,7 +18599,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-6271 - CCRU - KPI template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Convenience Big" sheetId="1" state="visible" r:id="rId2"/>
@@ -55,6 +55,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2558,19 +2559,19 @@
   </sheetPr>
   <dimension ref="A1:AR184"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G80" activeCellId="0" sqref="G80"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="AG149" activeCellId="0" sqref="AG149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="52.2753036437247"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="15.2834008097166"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="15.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="54.7004048582996"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="15.995951417004"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="15.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="15.995951417004"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="51.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15403,7 +15404,7 @@
         <v>0.0225</v>
       </c>
       <c r="AG148" s="38" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AH148" s="9" t="n">
         <v>1</v>
@@ -18430,7 +18431,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18467,7 +18468,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18599,7 +18600,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
PROS-6346 - CCRU - KPI template logic update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Convenience Big PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Convenience Big" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,6 +56,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Convenience Big'!$A$1:$AQ$172</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2727" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2731" uniqueCount="577">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -1324,6 +1325,12 @@
     <t xml:space="preserve">Сок Дисплей 1-й: Основной Добрый - Яблоко - 1л</t>
   </si>
   <si>
+    <t xml:space="preserve">Dobriy - Apple - 1L, Dobriy - Apple - 0.2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607042434877, 4607042430619</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dobriy - Apple - 1L share on Display</t>
   </si>
   <si>
@@ -1331,6 +1338,12 @@
   </si>
   <si>
     <t xml:space="preserve">Сок Дисплей 1-й: Основной Добрый - Мультифрут - 1л</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dobriy - Multifruit - 1L, Dobriy - Multifruit - 0.2L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4607042434891, 4607042430565</t>
   </si>
   <si>
     <t xml:space="preserve">Dobriy - Multifruit - 1L share on Display</t>
@@ -2009,7 +2022,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2092,6 +2105,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -2121,7 +2141,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2132,6 +2152,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -2198,7 +2224,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2227,8 +2253,11 @@
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2321,27 +2350,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2349,7 +2378,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2361,7 +2390,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2377,6 +2406,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2385,7 +2422,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2409,11 +2446,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2421,19 +2458,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2445,20 +2482,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
@@ -2466,6 +2503,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Good" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -2496,7 +2534,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
@@ -2521,7 +2559,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFC6EFCE"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -2559,19 +2597,19 @@
   </sheetPr>
   <dimension ref="A1:AR184"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="AG149" activeCellId="0" sqref="AG149"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="L147" activeCellId="0" sqref="L147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.95"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="15.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="54.7004048582996"/>
-    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="15.995951417004"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="15.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="15.995951417004"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="57.2712550607288"/>
+    <col collapsed="false" hidden="false" max="13" min="9" style="1" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="16.7125506072875"/>
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="51.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13850,11 +13888,11 @@
       <c r="K130" s="9"/>
       <c r="L130" s="9"/>
       <c r="M130" s="9"/>
-      <c r="N130" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="O130" s="16" t="n">
-        <v>4607042434877</v>
+      <c r="N130" s="37" t="s">
+        <v>386</v>
+      </c>
+      <c r="O130" s="38" t="s">
+        <v>387</v>
       </c>
       <c r="P130" s="16"/>
       <c r="Q130" s="16"/>
@@ -13891,7 +13929,7 @@
       <c r="AH130" s="9"/>
       <c r="AI130" s="9"/>
       <c r="AJ130" s="9" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="AK130" s="9"/>
       <c r="AL130" s="9"/>
@@ -13925,10 +13963,10 @@
       </c>
       <c r="F131" s="8"/>
       <c r="G131" s="9" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="H131" s="9" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="I131" s="9" t="s">
         <v>339</v>
@@ -13937,11 +13975,11 @@
       <c r="K131" s="9"/>
       <c r="L131" s="9"/>
       <c r="M131" s="9"/>
-      <c r="N131" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="O131" s="16" t="n">
-        <v>4607042434891</v>
+      <c r="N131" s="37" t="s">
+        <v>391</v>
+      </c>
+      <c r="O131" s="38" t="s">
+        <v>392</v>
       </c>
       <c r="P131" s="16"/>
       <c r="Q131" s="16"/>
@@ -13978,7 +14016,7 @@
       <c r="AH131" s="9"/>
       <c r="AI131" s="9"/>
       <c r="AJ131" s="9" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="AK131" s="9"/>
       <c r="AL131" s="9"/>
@@ -14012,10 +14050,10 @@
       </c>
       <c r="F132" s="8"/>
       <c r="G132" s="8" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="H132" s="8" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>327</v>
@@ -14063,7 +14101,7 @@
         <v>371</v>
       </c>
       <c r="AJ132" s="9" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="AK132" s="9"/>
       <c r="AL132" s="9"/>
@@ -14074,7 +14112,7 @@
         <v>131</v>
       </c>
       <c r="AO132" s="11" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="AP132" s="8"/>
       <c r="AQ132" s="8"/>
@@ -14097,10 +14135,10 @@
       </c>
       <c r="F133" s="8"/>
       <c r="G133" s="9" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="I133" s="9" t="s">
         <v>54</v>
@@ -14111,11 +14149,11 @@
       </c>
       <c r="L133" s="9"/>
       <c r="M133" s="9"/>
-      <c r="N133" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="O133" s="16" t="n">
-        <v>4607042434877</v>
+      <c r="N133" s="37" t="s">
+        <v>386</v>
+      </c>
+      <c r="O133" s="38" t="s">
+        <v>387</v>
       </c>
       <c r="P133" s="16"/>
       <c r="Q133" s="16"/>
@@ -14162,7 +14200,7 @@
       </c>
       <c r="AO133" s="8"/>
       <c r="AP133" s="8" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="AQ133" s="8"/>
     </row>
@@ -14184,10 +14222,10 @@
       </c>
       <c r="F134" s="8"/>
       <c r="G134" s="9" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="H134" s="9" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="I134" s="9" t="s">
         <v>54</v>
@@ -14198,11 +14236,11 @@
       </c>
       <c r="L134" s="9"/>
       <c r="M134" s="9"/>
-      <c r="N134" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="O134" s="16" t="n">
-        <v>4607042434891</v>
+      <c r="N134" s="37" t="s">
+        <v>391</v>
+      </c>
+      <c r="O134" s="38" t="s">
+        <v>392</v>
       </c>
       <c r="P134" s="16"/>
       <c r="Q134" s="16"/>
@@ -14249,7 +14287,7 @@
       </c>
       <c r="AO134" s="8"/>
       <c r="AP134" s="8" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="AQ134" s="8"/>
     </row>
@@ -14271,10 +14309,10 @@
       </c>
       <c r="F135" s="8"/>
       <c r="G135" s="9" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="I135" s="9" t="s">
         <v>54</v>
@@ -14336,7 +14374,7 @@
       </c>
       <c r="AO135" s="8"/>
       <c r="AP135" s="8" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="AQ135" s="8"/>
     </row>
@@ -14358,10 +14396,10 @@
       </c>
       <c r="F136" s="8"/>
       <c r="G136" s="9" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="H136" s="9" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="I136" s="9" t="s">
         <v>54</v>
@@ -14423,7 +14461,7 @@
       </c>
       <c r="AO136" s="8"/>
       <c r="AP136" s="8" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="AQ136" s="8"/>
     </row>
@@ -14445,10 +14483,10 @@
       </c>
       <c r="F137" s="8"/>
       <c r="G137" s="8" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="H137" s="8" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>327</v>
@@ -14472,7 +14510,7 @@
       <c r="V137" s="9"/>
       <c r="W137" s="8"/>
       <c r="X137" s="8" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="Y137" s="8"/>
       <c r="Z137" s="8"/>
@@ -14501,7 +14539,7 @@
         <v>136</v>
       </c>
       <c r="AO137" s="11" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="AP137" s="8"/>
       <c r="AQ137" s="8"/>
@@ -14524,10 +14562,10 @@
       </c>
       <c r="F138" s="8"/>
       <c r="G138" s="9" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="H138" s="9" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="I138" s="9" t="s">
         <v>54</v>
@@ -14559,7 +14597,7 @@
       <c r="V138" s="9"/>
       <c r="W138" s="8"/>
       <c r="X138" s="8" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="Y138" s="8"/>
       <c r="Z138" s="8"/>
@@ -14589,7 +14627,7 @@
       </c>
       <c r="AO138" s="8"/>
       <c r="AP138" s="8" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="AQ138" s="8"/>
     </row>
@@ -14611,10 +14649,10 @@
       </c>
       <c r="F139" s="8"/>
       <c r="G139" s="8" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="H139" s="8" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="I139" s="9" t="s">
         <v>334</v>
@@ -14638,11 +14676,11 @@
       <c r="T139" s="8"/>
       <c r="U139" s="8"/>
       <c r="V139" s="9" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="W139" s="8"/>
       <c r="X139" s="8" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="Y139" s="8"/>
       <c r="Z139" s="8"/>
@@ -14672,7 +14710,7 @@
       </c>
       <c r="AO139" s="8"/>
       <c r="AP139" s="8" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="AQ139" s="8"/>
     </row>
@@ -14694,10 +14732,10 @@
       </c>
       <c r="F140" s="8"/>
       <c r="G140" s="9" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="H140" s="9" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="I140" s="9" t="s">
         <v>382</v>
@@ -14721,7 +14759,7 @@
       <c r="V140" s="9"/>
       <c r="W140" s="8"/>
       <c r="X140" s="8" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="Y140" s="8"/>
       <c r="Z140" s="8"/>
@@ -14750,10 +14788,10 @@
         <v>139</v>
       </c>
       <c r="AO140" s="11" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="AP140" s="8" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="AQ140" s="8"/>
     </row>
@@ -14775,10 +14813,10 @@
       </c>
       <c r="F141" s="8"/>
       <c r="G141" s="9" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="H141" s="9" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="I141" s="9" t="s">
         <v>339</v>
@@ -14806,7 +14844,7 @@
       <c r="V141" s="9"/>
       <c r="W141" s="8"/>
       <c r="X141" s="8" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="Y141" s="8"/>
       <c r="Z141" s="8"/>
@@ -14826,7 +14864,7 @@
       <c r="AH141" s="9"/>
       <c r="AI141" s="9"/>
       <c r="AJ141" s="9" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="AK141" s="9"/>
       <c r="AL141" s="9"/>
@@ -14838,7 +14876,7 @@
       </c>
       <c r="AO141" s="8"/>
       <c r="AP141" s="8" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="AQ141" s="8"/>
     </row>
@@ -14860,10 +14898,10 @@
       </c>
       <c r="F142" s="8"/>
       <c r="G142" s="9" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="H142" s="9" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="I142" s="9" t="s">
         <v>339</v>
@@ -14891,7 +14929,7 @@
       <c r="V142" s="9"/>
       <c r="W142" s="8"/>
       <c r="X142" s="8" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="Y142" s="8"/>
       <c r="Z142" s="8"/>
@@ -14911,7 +14949,7 @@
       <c r="AH142" s="9"/>
       <c r="AI142" s="9"/>
       <c r="AJ142" s="9" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="AK142" s="9"/>
       <c r="AL142" s="9"/>
@@ -14923,7 +14961,7 @@
       </c>
       <c r="AO142" s="8"/>
       <c r="AP142" s="8" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="AQ142" s="8"/>
     </row>
@@ -14941,17 +14979,17 @@
         <v>45</v>
       </c>
       <c r="E143" s="8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="F143" s="8"/>
       <c r="G143" s="9" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="H143" s="8" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="I143" s="9" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="J143" s="9"/>
       <c r="K143" s="0"/>
@@ -14962,7 +15000,7 @@
       <c r="P143" s="22"/>
       <c r="Q143" s="22"/>
       <c r="R143" s="8" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="S143" s="8"/>
       <c r="T143" s="8"/>
@@ -14988,7 +15026,7 @@
       <c r="AH143" s="9"/>
       <c r="AI143" s="9"/>
       <c r="AJ143" s="9" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="AK143" s="9"/>
       <c r="AL143" s="9"/>
@@ -14999,7 +15037,7 @@
         <v>142</v>
       </c>
       <c r="AO143" s="11" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="AP143" s="8"/>
       <c r="AQ143" s="8"/>
@@ -15018,44 +15056,44 @@
         <v>45</v>
       </c>
       <c r="E144" s="8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="F144" s="8"/>
       <c r="G144" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="H144" s="9" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="J144" s="2"/>
       <c r="K144" s="9" t="n">
         <v>0.5</v>
       </c>
-      <c r="L144" s="9" t="n">
-        <v>28</v>
+      <c r="L144" s="38" t="n">
+        <v>24</v>
       </c>
       <c r="M144" s="9"/>
       <c r="N144" s="9" t="s">
         <v>251</v>
       </c>
       <c r="O144" s="10" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="P144" s="10"/>
       <c r="Q144" s="10"/>
       <c r="R144" s="8"/>
       <c r="S144" s="9" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="T144" s="8"/>
       <c r="U144" s="8"/>
       <c r="V144" s="8"/>
       <c r="W144" s="8"/>
       <c r="X144" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y144" s="8"/>
       <c r="Z144" s="8"/>
@@ -15085,7 +15123,7 @@
       </c>
       <c r="AO144" s="8"/>
       <c r="AP144" s="8" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="AQ144" s="8"/>
     </row>
@@ -15103,17 +15141,17 @@
         <v>45</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="F145" s="8"/>
       <c r="G145" s="9" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="H145" s="9" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="I145" s="9" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="J145" s="9"/>
       <c r="K145" s="9" t="n">
@@ -15125,20 +15163,20 @@
         <v>251</v>
       </c>
       <c r="O145" s="22" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="P145" s="22"/>
       <c r="Q145" s="22"/>
       <c r="R145" s="8"/>
       <c r="S145" s="8" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="T145" s="8"/>
       <c r="U145" s="8"/>
       <c r="V145" s="8"/>
       <c r="W145" s="8"/>
       <c r="X145" s="9" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="Y145" s="8"/>
       <c r="Z145" s="8"/>
@@ -15168,7 +15206,7 @@
       </c>
       <c r="AO145" s="8"/>
       <c r="AP145" s="8" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="AQ145" s="8"/>
     </row>
@@ -15190,10 +15228,10 @@
       </c>
       <c r="F146" s="8"/>
       <c r="G146" s="9" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="H146" s="12" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="I146" s="12" t="s">
         <v>334</v>
@@ -15210,16 +15248,16 @@
       <c r="Q146" s="22"/>
       <c r="R146" s="8"/>
       <c r="S146" s="1" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="T146" s="8"/>
       <c r="U146" s="8"/>
       <c r="V146" s="9" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="W146" s="8"/>
       <c r="X146" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y146" s="8"/>
       <c r="Z146" s="8"/>
@@ -15238,10 +15276,10 @@
       <c r="AG146" s="9"/>
       <c r="AH146" s="9"/>
       <c r="AI146" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ146" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK146" s="9"/>
       <c r="AL146" s="9"/>
@@ -15252,8 +15290,8 @@
         <v>145</v>
       </c>
       <c r="AO146" s="8"/>
-      <c r="AP146" s="37" t="s">
-        <v>442</v>
+      <c r="AP146" s="39" t="s">
+        <v>446</v>
       </c>
       <c r="AQ146" s="8"/>
     </row>
@@ -15275,13 +15313,13 @@
       </c>
       <c r="F147" s="8"/>
       <c r="G147" s="9" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="H147" s="9" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="J147" s="0"/>
       <c r="K147" s="2"/>
@@ -15304,7 +15342,7 @@
       <c r="V147" s="8"/>
       <c r="W147" s="8"/>
       <c r="X147" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y147" s="8"/>
       <c r="Z147" s="8"/>
@@ -15323,10 +15361,10 @@
       <c r="AG147" s="9"/>
       <c r="AH147" s="9"/>
       <c r="AI147" s="12" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ147" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK147" s="9"/>
       <c r="AL147" s="9"/>
@@ -15337,8 +15375,8 @@
         <v>146</v>
       </c>
       <c r="AO147" s="8"/>
-      <c r="AP147" s="37" t="s">
-        <v>442</v>
+      <c r="AP147" s="39" t="s">
+        <v>446</v>
       </c>
       <c r="AQ147" s="8"/>
     </row>
@@ -15360,10 +15398,10 @@
       </c>
       <c r="F148" s="8"/>
       <c r="G148" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="H148" s="9" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="I148" s="12" t="s">
         <v>260</v>
@@ -15387,7 +15425,7 @@
       <c r="V148" s="8"/>
       <c r="W148" s="8"/>
       <c r="X148" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y148" s="8"/>
       <c r="Z148" s="8"/>
@@ -15398,22 +15436,22 @@
         <v>50</v>
       </c>
       <c r="AE148" s="9" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="AF148" s="17" t="n">
         <v>0.0225</v>
       </c>
-      <c r="AG148" s="38" t="n">
+      <c r="AG148" s="40" t="n">
         <v>0.5</v>
       </c>
       <c r="AH148" s="9" t="n">
         <v>1</v>
       </c>
       <c r="AI148" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ148" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK148" s="9"/>
       <c r="AL148" s="9"/>
@@ -15424,10 +15462,10 @@
         <v>147</v>
       </c>
       <c r="AO148" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="AP148" s="37" t="s">
-        <v>442</v>
+        <v>453</v>
+      </c>
+      <c r="AP148" s="39" t="s">
+        <v>446</v>
       </c>
       <c r="AQ148" s="8"/>
     </row>
@@ -15449,10 +15487,10 @@
       </c>
       <c r="F149" s="8"/>
       <c r="G149" s="9" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="H149" s="9" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="I149" s="9" t="s">
         <v>54</v>
@@ -15482,7 +15520,7 @@
       <c r="V149" s="8"/>
       <c r="W149" s="8"/>
       <c r="X149" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y149" s="8"/>
       <c r="Z149" s="8"/>
@@ -15501,10 +15539,10 @@
       <c r="AG149" s="9"/>
       <c r="AH149" s="9"/>
       <c r="AI149" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ149" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK149" s="9"/>
       <c r="AL149" s="9"/>
@@ -15516,7 +15554,7 @@
       </c>
       <c r="AO149" s="8"/>
       <c r="AP149" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ149" s="8"/>
     </row>
@@ -15538,10 +15576,10 @@
       </c>
       <c r="F150" s="8"/>
       <c r="G150" s="9" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="H150" s="9" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="I150" s="9" t="s">
         <v>54</v>
@@ -15571,7 +15609,7 @@
       <c r="V150" s="8"/>
       <c r="W150" s="8"/>
       <c r="X150" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y150" s="8"/>
       <c r="Z150" s="8"/>
@@ -15590,10 +15628,10 @@
       <c r="AG150" s="9"/>
       <c r="AH150" s="9"/>
       <c r="AI150" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ150" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK150" s="9"/>
       <c r="AL150" s="9"/>
@@ -15605,7 +15643,7 @@
       </c>
       <c r="AO150" s="8"/>
       <c r="AP150" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ150" s="8"/>
     </row>
@@ -15627,10 +15665,10 @@
       </c>
       <c r="F151" s="8"/>
       <c r="G151" s="9" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="I151" s="9" t="s">
         <v>54</v>
@@ -15660,7 +15698,7 @@
       <c r="V151" s="8"/>
       <c r="W151" s="8"/>
       <c r="X151" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y151" s="8"/>
       <c r="Z151" s="8"/>
@@ -15679,10 +15717,10 @@
       <c r="AG151" s="9"/>
       <c r="AH151" s="9"/>
       <c r="AI151" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ151" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK151" s="9"/>
       <c r="AL151" s="9"/>
@@ -15694,7 +15732,7 @@
       </c>
       <c r="AO151" s="8"/>
       <c r="AP151" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ151" s="8"/>
     </row>
@@ -15716,10 +15754,10 @@
       </c>
       <c r="F152" s="8"/>
       <c r="G152" s="9" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="H152" s="9" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="I152" s="9" t="s">
         <v>54</v>
@@ -15749,7 +15787,7 @@
       <c r="V152" s="8"/>
       <c r="W152" s="8"/>
       <c r="X152" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y152" s="8"/>
       <c r="Z152" s="8"/>
@@ -15768,10 +15806,10 @@
       <c r="AG152" s="9"/>
       <c r="AH152" s="9"/>
       <c r="AI152" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ152" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK152" s="9"/>
       <c r="AL152" s="9"/>
@@ -15783,7 +15821,7 @@
       </c>
       <c r="AO152" s="8"/>
       <c r="AP152" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ152" s="8"/>
     </row>
@@ -15805,10 +15843,10 @@
       </c>
       <c r="F153" s="8"/>
       <c r="G153" s="9" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="H153" s="9" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="I153" s="9" t="s">
         <v>54</v>
@@ -15838,7 +15876,7 @@
       <c r="V153" s="8"/>
       <c r="W153" s="8"/>
       <c r="X153" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y153" s="8"/>
       <c r="Z153" s="8"/>
@@ -15857,10 +15895,10 @@
       <c r="AG153" s="9"/>
       <c r="AH153" s="9"/>
       <c r="AI153" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ153" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK153" s="9"/>
       <c r="AL153" s="9"/>
@@ -15872,7 +15910,7 @@
       </c>
       <c r="AO153" s="8"/>
       <c r="AP153" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ153" s="8"/>
     </row>
@@ -15894,10 +15932,10 @@
       </c>
       <c r="F154" s="8"/>
       <c r="G154" s="9" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="H154" s="9" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="I154" s="9" t="s">
         <v>54</v>
@@ -15927,7 +15965,7 @@
       <c r="V154" s="8"/>
       <c r="W154" s="8"/>
       <c r="X154" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y154" s="8"/>
       <c r="Z154" s="8"/>
@@ -15946,10 +15984,10 @@
       <c r="AG154" s="9"/>
       <c r="AH154" s="9"/>
       <c r="AI154" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ154" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK154" s="9"/>
       <c r="AL154" s="9"/>
@@ -15961,7 +15999,7 @@
       </c>
       <c r="AO154" s="8"/>
       <c r="AP154" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ154" s="8"/>
     </row>
@@ -15983,10 +16021,10 @@
       </c>
       <c r="F155" s="8"/>
       <c r="G155" s="9" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="H155" s="9" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="I155" s="9" t="s">
         <v>54</v>
@@ -16016,7 +16054,7 @@
       <c r="V155" s="8"/>
       <c r="W155" s="8"/>
       <c r="X155" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y155" s="8"/>
       <c r="Z155" s="8"/>
@@ -16035,10 +16073,10 @@
       <c r="AG155" s="9"/>
       <c r="AH155" s="9"/>
       <c r="AI155" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ155" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK155" s="9"/>
       <c r="AL155" s="9"/>
@@ -16050,7 +16088,7 @@
       </c>
       <c r="AO155" s="8"/>
       <c r="AP155" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ155" s="8"/>
     </row>
@@ -16072,10 +16110,10 @@
       </c>
       <c r="F156" s="8"/>
       <c r="G156" s="9" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="H156" s="9" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="I156" s="9" t="s">
         <v>54</v>
@@ -16105,7 +16143,7 @@
       <c r="V156" s="8"/>
       <c r="W156" s="8"/>
       <c r="X156" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y156" s="8"/>
       <c r="Z156" s="8"/>
@@ -16124,10 +16162,10 @@
       <c r="AG156" s="9"/>
       <c r="AH156" s="9"/>
       <c r="AI156" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ156" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK156" s="9"/>
       <c r="AL156" s="9"/>
@@ -16139,7 +16177,7 @@
       </c>
       <c r="AO156" s="8"/>
       <c r="AP156" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ156" s="8"/>
     </row>
@@ -16161,10 +16199,10 @@
       </c>
       <c r="F157" s="8"/>
       <c r="G157" s="9" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="H157" s="9" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="I157" s="9" t="s">
         <v>54</v>
@@ -16194,7 +16232,7 @@
       <c r="V157" s="8"/>
       <c r="W157" s="8"/>
       <c r="X157" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y157" s="8"/>
       <c r="Z157" s="8"/>
@@ -16213,10 +16251,10 @@
       <c r="AG157" s="9"/>
       <c r="AH157" s="9"/>
       <c r="AI157" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ157" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK157" s="9"/>
       <c r="AL157" s="9"/>
@@ -16228,7 +16266,7 @@
       </c>
       <c r="AO157" s="8"/>
       <c r="AP157" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ157" s="8"/>
     </row>
@@ -16250,10 +16288,10 @@
       </c>
       <c r="F158" s="8"/>
       <c r="G158" s="9" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="H158" s="9" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="I158" s="9" t="s">
         <v>54</v>
@@ -16283,7 +16321,7 @@
       <c r="V158" s="8"/>
       <c r="W158" s="8"/>
       <c r="X158" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y158" s="8"/>
       <c r="Z158" s="8"/>
@@ -16302,10 +16340,10 @@
       <c r="AG158" s="9"/>
       <c r="AH158" s="9"/>
       <c r="AI158" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ158" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK158" s="9"/>
       <c r="AL158" s="9"/>
@@ -16317,7 +16355,7 @@
       </c>
       <c r="AO158" s="8"/>
       <c r="AP158" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ158" s="8"/>
     </row>
@@ -16339,10 +16377,10 @@
       </c>
       <c r="F159" s="8"/>
       <c r="G159" s="9" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="H159" s="9" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="I159" s="9" t="s">
         <v>54</v>
@@ -16354,10 +16392,10 @@
       <c r="L159" s="9"/>
       <c r="M159" s="9"/>
       <c r="N159" s="9" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="O159" s="16" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="P159" s="22"/>
       <c r="Q159" s="22"/>
@@ -16372,7 +16410,7 @@
       <c r="V159" s="8"/>
       <c r="W159" s="8"/>
       <c r="X159" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y159" s="8"/>
       <c r="Z159" s="8"/>
@@ -16391,10 +16429,10 @@
       <c r="AG159" s="9"/>
       <c r="AH159" s="9"/>
       <c r="AI159" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ159" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK159" s="9"/>
       <c r="AL159" s="9"/>
@@ -16406,7 +16444,7 @@
       </c>
       <c r="AO159" s="8"/>
       <c r="AP159" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ159" s="8"/>
     </row>
@@ -16428,10 +16466,10 @@
       </c>
       <c r="F160" s="8"/>
       <c r="G160" s="9" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="H160" s="9" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="I160" s="9" t="s">
         <v>54</v>
@@ -16443,10 +16481,10 @@
       <c r="L160" s="9"/>
       <c r="M160" s="9"/>
       <c r="N160" s="9" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="O160" s="16" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="P160" s="22"/>
       <c r="Q160" s="22"/>
@@ -16461,7 +16499,7 @@
       <c r="V160" s="8"/>
       <c r="W160" s="8"/>
       <c r="X160" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y160" s="8"/>
       <c r="Z160" s="8"/>
@@ -16480,10 +16518,10 @@
       <c r="AG160" s="9"/>
       <c r="AH160" s="9"/>
       <c r="AI160" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ160" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK160" s="9"/>
       <c r="AL160" s="9"/>
@@ -16495,7 +16533,7 @@
       </c>
       <c r="AO160" s="8"/>
       <c r="AP160" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ160" s="8"/>
     </row>
@@ -16517,10 +16555,10 @@
       </c>
       <c r="F161" s="8"/>
       <c r="G161" s="9" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="H161" s="9" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="I161" s="9" t="s">
         <v>54</v>
@@ -16550,7 +16588,7 @@
       <c r="V161" s="8"/>
       <c r="W161" s="8"/>
       <c r="X161" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y161" s="8"/>
       <c r="Z161" s="8"/>
@@ -16569,10 +16607,10 @@
       <c r="AG161" s="9"/>
       <c r="AH161" s="9"/>
       <c r="AI161" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ161" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK161" s="9"/>
       <c r="AL161" s="9"/>
@@ -16584,7 +16622,7 @@
       </c>
       <c r="AO161" s="8"/>
       <c r="AP161" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ161" s="8"/>
     </row>
@@ -16606,10 +16644,10 @@
       </c>
       <c r="F162" s="8"/>
       <c r="G162" s="9" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="H162" s="9" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="I162" s="9" t="s">
         <v>54</v>
@@ -16639,7 +16677,7 @@
       <c r="V162" s="8"/>
       <c r="W162" s="8"/>
       <c r="X162" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y162" s="8"/>
       <c r="Z162" s="8"/>
@@ -16658,10 +16696,10 @@
       <c r="AG162" s="9"/>
       <c r="AH162" s="9"/>
       <c r="AI162" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ162" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK162" s="9"/>
       <c r="AL162" s="9"/>
@@ -16673,7 +16711,7 @@
       </c>
       <c r="AO162" s="8"/>
       <c r="AP162" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ162" s="8"/>
     </row>
@@ -16695,10 +16733,10 @@
       </c>
       <c r="F163" s="8"/>
       <c r="G163" s="9" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="H163" s="9" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="I163" s="9" t="s">
         <v>54</v>
@@ -16728,7 +16766,7 @@
       <c r="V163" s="8"/>
       <c r="W163" s="8"/>
       <c r="X163" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y163" s="8"/>
       <c r="Z163" s="8"/>
@@ -16747,10 +16785,10 @@
       <c r="AG163" s="9"/>
       <c r="AH163" s="9"/>
       <c r="AI163" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ163" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK163" s="9"/>
       <c r="AL163" s="9"/>
@@ -16762,7 +16800,7 @@
       </c>
       <c r="AO163" s="8"/>
       <c r="AP163" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ163" s="8"/>
     </row>
@@ -16784,10 +16822,10 @@
       </c>
       <c r="F164" s="8"/>
       <c r="G164" s="9" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="H164" s="9" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="I164" s="9" t="s">
         <v>54</v>
@@ -16817,7 +16855,7 @@
       <c r="V164" s="8"/>
       <c r="W164" s="8"/>
       <c r="X164" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y164" s="8"/>
       <c r="Z164" s="8"/>
@@ -16836,10 +16874,10 @@
       <c r="AG164" s="9"/>
       <c r="AH164" s="9"/>
       <c r="AI164" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ164" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK164" s="9"/>
       <c r="AL164" s="9"/>
@@ -16851,7 +16889,7 @@
       </c>
       <c r="AO164" s="8"/>
       <c r="AP164" s="9" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="AQ164" s="8"/>
     </row>
@@ -16873,13 +16911,13 @@
       </c>
       <c r="F165" s="8"/>
       <c r="G165" s="9" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="H165" s="8" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="I165" s="12" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="J165" s="12"/>
       <c r="K165" s="9"/>
@@ -16889,20 +16927,20 @@
         <v>251</v>
       </c>
       <c r="O165" s="10" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="P165" s="10"/>
       <c r="Q165" s="10"/>
       <c r="R165" s="8"/>
       <c r="S165" s="8" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="T165" s="9"/>
       <c r="U165" s="9"/>
       <c r="V165" s="8"/>
       <c r="W165" s="8"/>
       <c r="X165" s="9" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="Y165" s="9"/>
       <c r="Z165" s="8"/>
@@ -16921,10 +16959,10 @@
       <c r="AG165" s="9"/>
       <c r="AH165" s="9"/>
       <c r="AI165" s="9" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AJ165" s="9" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK165" s="9"/>
       <c r="AL165" s="9"/>
@@ -16935,8 +16973,8 @@
         <v>164</v>
       </c>
       <c r="AO165" s="8"/>
-      <c r="AP165" s="37" t="s">
-        <v>442</v>
+      <c r="AP165" s="39" t="s">
+        <v>446</v>
       </c>
       <c r="AQ165" s="8"/>
     </row>
@@ -16953,18 +16991,18 @@
       <c r="D166" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="E166" s="39" t="s">
+      <c r="E166" s="41" t="s">
         <v>257</v>
       </c>
-      <c r="F166" s="39"/>
+      <c r="F166" s="41"/>
       <c r="G166" s="9" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="H166" s="8" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="I166" s="9" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="J166" s="9"/>
       <c r="K166" s="9" t="n">
@@ -16985,7 +17023,7 @@
       <c r="V166" s="9"/>
       <c r="W166" s="9"/>
       <c r="X166" s="9" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="Y166" s="9"/>
       <c r="Z166" s="9"/>
@@ -17014,10 +17052,10 @@
         <v>165</v>
       </c>
       <c r="AO166" s="35" t="s">
-        <v>491</v>
-      </c>
-      <c r="AP166" s="37" t="s">
-        <v>492</v>
+        <v>495</v>
+      </c>
+      <c r="AP166" s="39" t="s">
+        <v>496</v>
       </c>
       <c r="AQ166" s="8"/>
     </row>
@@ -17034,18 +17072,18 @@
       <c r="D167" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="E167" s="39" t="s">
+      <c r="E167" s="41" t="s">
         <v>257</v>
       </c>
-      <c r="F167" s="39"/>
+      <c r="F167" s="41"/>
       <c r="G167" s="9" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="H167" s="8" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="J167" s="0"/>
       <c r="K167" s="1" t="n">
@@ -17059,7 +17097,7 @@
         <v>251</v>
       </c>
       <c r="O167" s="10" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="P167" s="10"/>
       <c r="Q167" s="10"/>
@@ -17067,14 +17105,14 @@
         <v>55</v>
       </c>
       <c r="S167" s="1" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="T167" s="9"/>
       <c r="U167" s="9"/>
       <c r="V167" s="9"/>
       <c r="W167" s="9"/>
       <c r="X167" s="9" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="Y167" s="9"/>
       <c r="Z167" s="9"/>
@@ -17085,7 +17123,7 @@
         <v>50</v>
       </c>
       <c r="AE167" s="9" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="AF167" s="17" t="n">
         <v>1</v>
@@ -17094,7 +17132,7 @@
       <c r="AH167" s="9"/>
       <c r="AI167" s="9"/>
       <c r="AJ167" s="9" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="AK167" s="9"/>
       <c r="AL167" s="9"/>
@@ -17106,7 +17144,7 @@
       </c>
       <c r="AO167" s="8"/>
       <c r="AP167" s="12" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="AQ167" s="8"/>
     </row>
@@ -17128,10 +17166,10 @@
       </c>
       <c r="F168" s="8"/>
       <c r="G168" s="9" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="H168" s="8" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="I168" s="9" t="s">
         <v>260</v>
@@ -17182,10 +17220,10 @@
         <v>167</v>
       </c>
       <c r="AO168" s="11" t="s">
-        <v>500</v>
-      </c>
-      <c r="AP168" s="40" t="s">
-        <v>501</v>
+        <v>504</v>
+      </c>
+      <c r="AP168" s="42" t="s">
+        <v>505</v>
       </c>
       <c r="AQ168" s="8"/>
     </row>
@@ -17207,10 +17245,10 @@
       </c>
       <c r="F169" s="8"/>
       <c r="G169" s="9" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="H169" s="8" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
       <c r="I169" s="8" t="s">
         <v>334</v>
@@ -17236,8 +17274,8 @@
       <c r="V169" s="9"/>
       <c r="W169" s="9"/>
       <c r="X169" s="9"/>
-      <c r="Y169" s="41" t="s">
-        <v>504</v>
+      <c r="Y169" s="43" t="s">
+        <v>508</v>
       </c>
       <c r="Z169" s="9"/>
       <c r="AA169" s="8"/>
@@ -17266,7 +17304,7 @@
       </c>
       <c r="AO169" s="9"/>
       <c r="AP169" s="9" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="AQ169" s="8"/>
     </row>
@@ -17288,10 +17326,10 @@
       </c>
       <c r="F170" s="8"/>
       <c r="G170" s="9" t="s">
-        <v>505</v>
+        <v>509</v>
       </c>
       <c r="H170" s="8" t="s">
-        <v>506</v>
+        <v>510</v>
       </c>
       <c r="I170" s="8" t="s">
         <v>334</v>
@@ -17318,7 +17356,7 @@
       <c r="W170" s="9"/>
       <c r="X170" s="9"/>
       <c r="Y170" s="9" t="s">
-        <v>507</v>
+        <v>511</v>
       </c>
       <c r="Z170" s="9"/>
       <c r="AA170" s="8"/>
@@ -17347,7 +17385,7 @@
       </c>
       <c r="AO170" s="9"/>
       <c r="AP170" s="9" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="AQ170" s="8"/>
     </row>
@@ -17369,10 +17407,10 @@
       </c>
       <c r="F171" s="8"/>
       <c r="G171" s="9" t="s">
-        <v>508</v>
+        <v>512</v>
       </c>
       <c r="H171" s="8" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="I171" s="8" t="s">
         <v>334</v>
@@ -17399,7 +17437,7 @@
       <c r="W171" s="9"/>
       <c r="X171" s="9"/>
       <c r="Y171" s="9" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="Z171" s="9"/>
       <c r="AA171" s="8"/>
@@ -17428,7 +17466,7 @@
       </c>
       <c r="AO171" s="9"/>
       <c r="AP171" s="9" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="AQ171" s="8"/>
     </row>
@@ -17450,10 +17488,10 @@
       </c>
       <c r="F172" s="8"/>
       <c r="G172" s="9" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="H172" s="8" t="s">
-        <v>512</v>
+        <v>516</v>
       </c>
       <c r="I172" s="8" t="s">
         <v>334</v>
@@ -17480,7 +17518,7 @@
       <c r="W172" s="9"/>
       <c r="X172" s="9"/>
       <c r="Y172" s="9" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="Z172" s="9"/>
       <c r="AA172" s="8"/>
@@ -17509,7 +17547,7 @@
       </c>
       <c r="AO172" s="9"/>
       <c r="AP172" s="9" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
       <c r="AQ172" s="8"/>
     </row>
@@ -17523,24 +17561,24 @@
       <c r="C173" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D173" s="42" t="s">
-        <v>514</v>
+      <c r="D173" s="44" t="s">
+        <v>518</v>
       </c>
       <c r="E173" s="32" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="F173" s="32" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="G173" s="14" t="s">
         <v>264</v>
       </c>
       <c r="H173" s="14"/>
       <c r="I173" s="8" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="J173" s="8" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="K173" s="8"/>
       <c r="L173" s="8"/>
@@ -17551,7 +17589,7 @@
       <c r="Q173" s="8"/>
       <c r="R173" s="8"/>
       <c r="S173" s="8" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="T173" s="8"/>
       <c r="U173" s="8"/>
@@ -17565,7 +17603,7 @@
       <c r="AC173" s="8"/>
       <c r="AD173" s="8"/>
       <c r="AE173" s="8"/>
-      <c r="AF173" s="43" t="n">
+      <c r="AF173" s="45" t="n">
         <v>0</v>
       </c>
       <c r="AG173" s="8"/>
@@ -17579,7 +17617,7 @@
         <v>172</v>
       </c>
       <c r="AO173" s="9" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="AP173" s="8"/>
       <c r="AQ173" s="8"/>
@@ -17594,24 +17632,24 @@
       <c r="C174" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D174" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E174" s="37" t="s">
-        <v>521</v>
-      </c>
-      <c r="F174" s="37" t="s">
-        <v>522</v>
-      </c>
-      <c r="G174" s="40" t="s">
-        <v>501</v>
+      <c r="D174" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E174" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="F174" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="G174" s="42" t="s">
+        <v>505</v>
       </c>
       <c r="H174" s="8"/>
       <c r="I174" s="8" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="J174" s="8" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="K174" s="8"/>
       <c r="L174" s="8"/>
@@ -17622,7 +17660,7 @@
       <c r="Q174" s="8"/>
       <c r="R174" s="8"/>
       <c r="S174" s="8" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="T174" s="8"/>
       <c r="U174" s="8"/>
@@ -17636,7 +17674,7 @@
       <c r="AC174" s="8"/>
       <c r="AD174" s="8"/>
       <c r="AE174" s="8"/>
-      <c r="AF174" s="44" t="n">
+      <c r="AF174" s="46" t="n">
         <v>0</v>
       </c>
       <c r="AG174" s="8"/>
@@ -17665,24 +17703,24 @@
       <c r="C175" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D175" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E175" s="37" t="s">
-        <v>524</v>
-      </c>
-      <c r="F175" s="37" t="s">
-        <v>525</v>
-      </c>
-      <c r="G175" s="37" t="s">
-        <v>442</v>
+      <c r="D175" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E175" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="F175" s="39" t="s">
+        <v>529</v>
+      </c>
+      <c r="G175" s="39" t="s">
+        <v>446</v>
       </c>
       <c r="H175" s="8"/>
       <c r="I175" s="8" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="J175" s="8" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="K175" s="8"/>
       <c r="L175" s="8"/>
@@ -17693,7 +17731,7 @@
       <c r="Q175" s="8"/>
       <c r="R175" s="8"/>
       <c r="S175" s="8" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="T175" s="8"/>
       <c r="U175" s="8"/>
@@ -17707,7 +17745,7 @@
       <c r="AC175" s="8"/>
       <c r="AD175" s="8"/>
       <c r="AE175" s="8"/>
-      <c r="AF175" s="43" t="n">
+      <c r="AF175" s="45" t="n">
         <v>0</v>
       </c>
       <c r="AG175" s="8"/>
@@ -17721,7 +17759,7 @@
         <v>174</v>
       </c>
       <c r="AO175" s="9" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="AP175" s="8"/>
       <c r="AQ175" s="8"/>
@@ -17736,24 +17774,24 @@
       <c r="C176" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D176" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E176" s="37" t="s">
-        <v>529</v>
-      </c>
-      <c r="F176" s="37" t="s">
-        <v>530</v>
-      </c>
-      <c r="G176" s="37" t="s">
-        <v>492</v>
+      <c r="D176" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E176" s="39" t="s">
+        <v>533</v>
+      </c>
+      <c r="F176" s="39" t="s">
+        <v>534</v>
+      </c>
+      <c r="G176" s="39" t="s">
+        <v>496</v>
       </c>
       <c r="H176" s="8"/>
       <c r="I176" s="8" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="J176" s="8" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="K176" s="8"/>
       <c r="L176" s="8"/>
@@ -17764,7 +17802,7 @@
       <c r="Q176" s="8"/>
       <c r="R176" s="8"/>
       <c r="S176" s="8" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="T176" s="8"/>
       <c r="U176" s="8"/>
@@ -17778,7 +17816,7 @@
       <c r="AC176" s="8"/>
       <c r="AD176" s="8"/>
       <c r="AE176" s="8"/>
-      <c r="AF176" s="43" t="n">
+      <c r="AF176" s="45" t="n">
         <v>0</v>
       </c>
       <c r="AG176" s="8"/>
@@ -17807,24 +17845,24 @@
       <c r="C177" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D177" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E177" s="37" t="s">
-        <v>531</v>
-      </c>
-      <c r="F177" s="37" t="s">
-        <v>532</v>
-      </c>
-      <c r="G177" s="37" t="s">
-        <v>533</v>
+      <c r="D177" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E177" s="39" t="s">
+        <v>535</v>
+      </c>
+      <c r="F177" s="39" t="s">
+        <v>536</v>
+      </c>
+      <c r="G177" s="39" t="s">
+        <v>537</v>
       </c>
       <c r="H177" s="8"/>
       <c r="I177" s="9" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="J177" s="9" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="K177" s="8"/>
       <c r="L177" s="8"/>
@@ -17835,7 +17873,7 @@
       <c r="Q177" s="8"/>
       <c r="R177" s="8"/>
       <c r="S177" s="8" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="T177" s="8"/>
       <c r="U177" s="8"/>
@@ -17849,7 +17887,7 @@
       <c r="AC177" s="8"/>
       <c r="AD177" s="8"/>
       <c r="AE177" s="8"/>
-      <c r="AF177" s="43" t="n">
+      <c r="AF177" s="45" t="n">
         <v>0</v>
       </c>
       <c r="AG177" s="8"/>
@@ -17863,7 +17901,7 @@
         <v>176</v>
       </c>
       <c r="AO177" s="9" t="s">
-        <v>534</v>
+        <v>538</v>
       </c>
       <c r="AP177" s="8"/>
       <c r="AQ177" s="8"/>
@@ -17878,37 +17916,37 @@
       <c r="C178" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D178" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E178" s="37" t="s">
-        <v>535</v>
-      </c>
-      <c r="F178" s="37" t="s">
-        <v>536</v>
-      </c>
-      <c r="G178" s="37" t="s">
-        <v>537</v>
+      <c r="D178" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E178" s="39" t="s">
+        <v>539</v>
+      </c>
+      <c r="F178" s="39" t="s">
+        <v>540</v>
+      </c>
+      <c r="G178" s="39" t="s">
+        <v>541</v>
       </c>
       <c r="H178" s="8"/>
       <c r="I178" s="9" t="s">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="J178" s="9" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="K178" s="8"/>
       <c r="L178" s="8"/>
       <c r="M178" s="9"/>
       <c r="N178" s="9"/>
       <c r="O178" s="8" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
       <c r="P178" s="8"/>
       <c r="Q178" s="8"/>
       <c r="R178" s="8"/>
       <c r="S178" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="T178" s="8"/>
       <c r="U178" s="8"/>
@@ -17916,7 +17954,7 @@
       <c r="W178" s="8"/>
       <c r="X178" s="8"/>
       <c r="Y178" s="9" t="s">
-        <v>541</v>
+        <v>545</v>
       </c>
       <c r="Z178" s="8"/>
       <c r="AA178" s="8"/>
@@ -17951,24 +17989,24 @@
       <c r="C179" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D179" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E179" s="37" t="s">
-        <v>542</v>
-      </c>
-      <c r="F179" s="37" t="s">
-        <v>543</v>
-      </c>
-      <c r="G179" s="37" t="s">
-        <v>544</v>
+      <c r="D179" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E179" s="39" t="s">
+        <v>546</v>
+      </c>
+      <c r="F179" s="39" t="s">
+        <v>547</v>
+      </c>
+      <c r="G179" s="39" t="s">
+        <v>548</v>
       </c>
       <c r="H179" s="8"/>
       <c r="I179" s="9" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="J179" s="9" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="K179" s="8"/>
       <c r="L179" s="8"/>
@@ -17981,7 +18019,7 @@
       <c r="Q179" s="8"/>
       <c r="R179" s="8"/>
       <c r="S179" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="T179" s="8"/>
       <c r="U179" s="8"/>
@@ -17989,7 +18027,7 @@
       <c r="W179" s="8"/>
       <c r="X179" s="8"/>
       <c r="Y179" s="9" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="Z179" s="8"/>
       <c r="AA179" s="8"/>
@@ -18024,37 +18062,37 @@
       <c r="C180" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D180" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E180" s="37" t="s">
-        <v>548</v>
-      </c>
-      <c r="F180" s="37" t="s">
-        <v>549</v>
-      </c>
-      <c r="G180" s="37" t="s">
-        <v>550</v>
+      <c r="D180" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E180" s="39" t="s">
+        <v>552</v>
+      </c>
+      <c r="F180" s="39" t="s">
+        <v>553</v>
+      </c>
+      <c r="G180" s="39" t="s">
+        <v>554</v>
       </c>
       <c r="H180" s="8"/>
       <c r="I180" s="9" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="J180" s="9" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="K180" s="8"/>
       <c r="L180" s="8"/>
       <c r="M180" s="9"/>
       <c r="N180" s="9"/>
       <c r="O180" s="8" t="s">
-        <v>551</v>
+        <v>555</v>
       </c>
       <c r="P180" s="8"/>
       <c r="Q180" s="8"/>
       <c r="R180" s="8"/>
       <c r="S180" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="T180" s="8"/>
       <c r="U180" s="8"/>
@@ -18062,7 +18100,7 @@
       <c r="W180" s="8"/>
       <c r="X180" s="8"/>
       <c r="Y180" s="9" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="Z180" s="8"/>
       <c r="AA180" s="8"/>
@@ -18097,39 +18135,39 @@
       <c r="C181" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D181" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E181" s="37" t="s">
-        <v>552</v>
-      </c>
-      <c r="F181" s="37" t="s">
-        <v>553</v>
-      </c>
-      <c r="G181" s="37" t="s">
-        <v>554</v>
+      <c r="D181" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E181" s="39" t="s">
+        <v>556</v>
+      </c>
+      <c r="F181" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="G181" s="39" t="s">
+        <v>558</v>
       </c>
       <c r="H181" s="8" t="s">
         <v>325</v>
       </c>
       <c r="I181" s="9" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="J181" s="9" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="K181" s="8"/>
       <c r="L181" s="8"/>
       <c r="M181" s="9"/>
       <c r="N181" s="9"/>
       <c r="O181" s="9" t="s">
-        <v>556</v>
+        <v>560</v>
       </c>
       <c r="P181" s="8"/>
       <c r="Q181" s="8"/>
       <c r="R181" s="8"/>
       <c r="S181" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="T181" s="8"/>
       <c r="U181" s="8"/>
@@ -18137,7 +18175,7 @@
       <c r="W181" s="8"/>
       <c r="X181" s="8"/>
       <c r="Y181" s="9" t="s">
-        <v>557</v>
+        <v>561</v>
       </c>
       <c r="Z181" s="8"/>
       <c r="AA181" s="8"/>
@@ -18174,39 +18212,39 @@
       <c r="C182" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D182" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E182" s="37" t="s">
-        <v>552</v>
-      </c>
-      <c r="F182" s="37" t="s">
-        <v>553</v>
-      </c>
-      <c r="G182" s="37" t="s">
-        <v>554</v>
+      <c r="D182" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E182" s="39" t="s">
+        <v>556</v>
+      </c>
+      <c r="F182" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="G182" s="39" t="s">
+        <v>558</v>
       </c>
       <c r="H182" s="8" t="s">
         <v>351</v>
       </c>
       <c r="I182" s="9" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="J182" s="9" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="K182" s="8"/>
       <c r="L182" s="8"/>
       <c r="M182" s="9"/>
       <c r="N182" s="9"/>
       <c r="O182" s="9" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="P182" s="8"/>
       <c r="Q182" s="8"/>
       <c r="R182" s="8"/>
       <c r="S182" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="T182" s="8"/>
       <c r="U182" s="8"/>
@@ -18214,7 +18252,7 @@
       <c r="W182" s="8"/>
       <c r="X182" s="8"/>
       <c r="Y182" s="9" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="Z182" s="8"/>
       <c r="AA182" s="8"/>
@@ -18251,39 +18289,39 @@
       <c r="C183" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D183" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E183" s="37" t="s">
-        <v>552</v>
-      </c>
-      <c r="F183" s="37" t="s">
-        <v>553</v>
-      </c>
-      <c r="G183" s="37" t="s">
-        <v>554</v>
+      <c r="D183" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E183" s="39" t="s">
+        <v>556</v>
+      </c>
+      <c r="F183" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="G183" s="39" t="s">
+        <v>558</v>
       </c>
       <c r="H183" s="8" t="s">
         <v>371</v>
       </c>
       <c r="I183" s="9" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="J183" s="9" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="K183" s="8"/>
       <c r="L183" s="8"/>
       <c r="M183" s="9"/>
       <c r="N183" s="9"/>
       <c r="O183" s="9" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="P183" s="8"/>
       <c r="Q183" s="8"/>
       <c r="R183" s="8"/>
       <c r="S183" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="T183" s="8"/>
       <c r="U183" s="8"/>
@@ -18291,7 +18329,7 @@
       <c r="W183" s="8"/>
       <c r="X183" s="8"/>
       <c r="Y183" s="9" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="Z183" s="8"/>
       <c r="AA183" s="8"/>
@@ -18328,39 +18366,39 @@
       <c r="C184" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D184" s="42" t="s">
-        <v>514</v>
-      </c>
-      <c r="E184" s="37" t="s">
-        <v>552</v>
-      </c>
-      <c r="F184" s="37" t="s">
-        <v>553</v>
-      </c>
-      <c r="G184" s="37" t="s">
-        <v>554</v>
+      <c r="D184" s="44" t="s">
+        <v>518</v>
+      </c>
+      <c r="E184" s="39" t="s">
+        <v>556</v>
+      </c>
+      <c r="F184" s="39" t="s">
+        <v>557</v>
+      </c>
+      <c r="G184" s="39" t="s">
+        <v>558</v>
       </c>
       <c r="H184" s="8" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="I184" s="9" t="s">
-        <v>555</v>
+        <v>559</v>
       </c>
       <c r="J184" s="9" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="K184" s="8"/>
       <c r="L184" s="8"/>
       <c r="M184" s="9"/>
       <c r="N184" s="9"/>
       <c r="O184" s="9" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="P184" s="8"/>
       <c r="Q184" s="8"/>
       <c r="R184" s="8"/>
       <c r="S184" s="8" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
       <c r="T184" s="8"/>
       <c r="U184" s="8"/>
@@ -18368,7 +18406,7 @@
       <c r="W184" s="8"/>
       <c r="X184" s="8"/>
       <c r="Y184" s="9" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="Z184" s="8"/>
       <c r="AA184" s="8"/>
@@ -18430,18 +18468,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="45" t="s">
-        <v>504</v>
+      <c r="A1" s="47" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="165" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="46" t="s">
-        <v>441</v>
+      <c r="A2" s="48" t="s">
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -18467,41 +18502,38 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="47" t="s">
-        <v>427</v>
+      <c r="B1" s="49" t="s">
+        <v>431</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="H1" s="47" t="s">
-        <v>486</v>
+        <v>570</v>
+      </c>
+      <c r="H1" s="49" t="s">
+        <v>490</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="47"/>
+      <c r="B2" s="49"/>
       <c r="C2" s="0" t="n">
         <v>0.7</v>
       </c>
@@ -18509,19 +18541,19 @@
         <f aca="false">C2*$C$6</f>
         <v>19.6</v>
       </c>
-      <c r="E2" s="48" t="n">
+      <c r="E2" s="50" t="n">
         <v>20</v>
       </c>
-      <c r="H2" s="47"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="0" t="n">
         <v>0.7</v>
       </c>
-      <c r="J2" s="49" t="n">
+      <c r="J2" s="51" t="n">
         <v>0.99</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="47"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="0" t="n">
         <v>1</v>
       </c>
@@ -18529,19 +18561,19 @@
         <f aca="false">C3*$C$6</f>
         <v>28</v>
       </c>
-      <c r="E3" s="50" t="n">
+      <c r="E3" s="52" t="n">
         <v>22</v>
       </c>
-      <c r="H3" s="47"/>
+      <c r="H3" s="49"/>
       <c r="I3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="J3" s="51" t="n">
+      <c r="J3" s="53" t="n">
         <v>0.8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="47"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
@@ -18549,28 +18581,28 @@
         <f aca="false">C4*$C$6</f>
         <v>56</v>
       </c>
-      <c r="E4" s="50" t="n">
+      <c r="E4" s="52" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="52" t="n">
+      <c r="F4" s="54" t="n">
         <f aca="false">C2/SUM(C2:C4)</f>
         <v>0.189189189189189</v>
       </c>
-      <c r="H4" s="47"/>
+      <c r="H4" s="49"/>
       <c r="I4" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="49" t="n">
+      <c r="J4" s="51" t="n">
         <v>0.99</v>
       </c>
-      <c r="K4" s="53" t="n">
+      <c r="K4" s="55" t="n">
         <f aca="false">SUM(I2,I4)/SUM(I2:I4)</f>
         <v>0.72972972972973</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>28</v>
@@ -18599,54 +18631,51 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.57085020242915"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="55" t="s">
-        <v>569</v>
-      </c>
-      <c r="H1" s="55" t="s">
-        <v>570</v>
-      </c>
-      <c r="I1" s="55" t="s">
+      <c r="G1" s="57" t="s">
+        <v>573</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>574</v>
+      </c>
+      <c r="I1" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="55" t="s">
-        <v>571</v>
-      </c>
-      <c r="L1" s="55" t="s">
+      <c r="K1" s="57" t="s">
+        <v>575</v>
+      </c>
+      <c r="L1" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="57" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="56" t="s">
-        <v>572</v>
+      <c r="B4" s="58" t="s">
+        <v>576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>